<commit_message>
Se unifica los dataframe de COESTI y Externos con todo el software
</commit_message>
<xml_diff>
--- a/datos_intermedios/Data_Filtrada_COESTI.xlsx
+++ b/datos_intermedios/Data_Filtrada_COESTI.xlsx
@@ -524,8 +524,10 @@
       <c r="G2" t="n">
         <v>4500</v>
       </c>
-      <c r="H2" t="n">
-        <v>40002019</v>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>40002019</t>
+        </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
@@ -577,8 +579,10 @@
       <c r="G3" t="n">
         <v>4000</v>
       </c>
-      <c r="H3" t="n">
-        <v>40002019</v>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>40002019</t>
+        </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
@@ -630,8 +634,10 @@
       <c r="G4" t="n">
         <v>500</v>
       </c>
-      <c r="H4" t="n">
-        <v>40002047</v>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>40002047</t>
+        </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
@@ -683,8 +689,10 @@
       <c r="G5" t="n">
         <v>2500</v>
       </c>
-      <c r="H5" t="n">
-        <v>40002019</v>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>40002019</t>
+        </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
@@ -736,8 +744,10 @@
       <c r="G6" t="n">
         <v>500</v>
       </c>
-      <c r="H6" t="n">
-        <v>40002039</v>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>40002039</t>
+        </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
@@ -789,8 +799,10 @@
       <c r="G7" t="n">
         <v>4000</v>
       </c>
-      <c r="H7" t="n">
-        <v>40002019</v>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>40002019</t>
+        </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
@@ -842,8 +854,10 @@
       <c r="G8" t="n">
         <v>3000</v>
       </c>
-      <c r="H8" t="n">
-        <v>40002039</v>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>40002039</t>
+        </is>
       </c>
       <c r="I8" t="inlineStr">
         <is>
@@ -895,8 +909,10 @@
       <c r="G9" t="n">
         <v>2000</v>
       </c>
-      <c r="H9" t="n">
-        <v>40002047</v>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>40002047</t>
+        </is>
       </c>
       <c r="I9" t="inlineStr">
         <is>
@@ -948,8 +964,10 @@
       <c r="G10" t="n">
         <v>1000</v>
       </c>
-      <c r="H10" t="n">
-        <v>40002039</v>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>40002039</t>
+        </is>
       </c>
       <c r="I10" t="inlineStr">
         <is>
@@ -1001,8 +1019,10 @@
       <c r="G11" t="n">
         <v>2500</v>
       </c>
-      <c r="H11" t="n">
-        <v>40002047</v>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>40002047</t>
+        </is>
       </c>
       <c r="I11" t="inlineStr">
         <is>
@@ -1054,8 +1074,10 @@
       <c r="G12" t="n">
         <v>500</v>
       </c>
-      <c r="H12" t="n">
-        <v>40002055</v>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>40002055</t>
+        </is>
       </c>
       <c r="I12" t="inlineStr">
         <is>
@@ -1107,8 +1129,10 @@
       <c r="G13" t="n">
         <v>1500</v>
       </c>
-      <c r="H13" t="n">
-        <v>40002019</v>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>40002019</t>
+        </is>
       </c>
       <c r="I13" t="inlineStr">
         <is>
@@ -1160,8 +1184,10 @@
       <c r="G14" t="n">
         <v>2000</v>
       </c>
-      <c r="H14" t="n">
-        <v>40002039</v>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>40002039</t>
+        </is>
       </c>
       <c r="I14" t="inlineStr">
         <is>
@@ -1213,8 +1239,10 @@
       <c r="G15" t="n">
         <v>1000</v>
       </c>
-      <c r="H15" t="n">
-        <v>40002047</v>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>40002047</t>
+        </is>
       </c>
       <c r="I15" t="inlineStr">
         <is>
@@ -1266,8 +1294,10 @@
       <c r="G16" t="n">
         <v>2500</v>
       </c>
-      <c r="H16" t="n">
-        <v>40002019</v>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>40002019</t>
+        </is>
       </c>
       <c r="I16" t="inlineStr">
         <is>
@@ -1319,8 +1349,10 @@
       <c r="G17" t="n">
         <v>500</v>
       </c>
-      <c r="H17" t="n">
-        <v>40002039</v>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>40002039</t>
+        </is>
       </c>
       <c r="I17" t="inlineStr">
         <is>
@@ -1372,8 +1404,10 @@
       <c r="G18" t="n">
         <v>7000</v>
       </c>
-      <c r="H18" t="n">
-        <v>40002019</v>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>40002019</t>
+        </is>
       </c>
       <c r="I18" t="inlineStr">
         <is>
@@ -1425,8 +1459,10 @@
       <c r="G19" t="n">
         <v>2000</v>
       </c>
-      <c r="H19" t="n">
-        <v>40002047</v>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>40002047</t>
+        </is>
       </c>
       <c r="I19" t="inlineStr">
         <is>
@@ -1478,8 +1514,10 @@
       <c r="G20" t="n">
         <v>1000</v>
       </c>
-      <c r="H20" t="n">
-        <v>40002019</v>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>40002019</t>
+        </is>
       </c>
       <c r="I20" t="inlineStr">
         <is>
@@ -1531,8 +1569,10 @@
       <c r="G21" t="n">
         <v>500</v>
       </c>
-      <c r="H21" t="n">
-        <v>40002047</v>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>40002047</t>
+        </is>
       </c>
       <c r="I21" t="inlineStr">
         <is>
@@ -1584,8 +1624,10 @@
       <c r="G22" t="n">
         <v>1000</v>
       </c>
-      <c r="H22" t="n">
-        <v>40002055</v>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>40002055</t>
+        </is>
       </c>
       <c r="I22" t="inlineStr">
         <is>
@@ -1637,8 +1679,10 @@
       <c r="G23" t="n">
         <v>2000</v>
       </c>
-      <c r="H23" t="n">
-        <v>40002019</v>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>40002019</t>
+        </is>
       </c>
       <c r="I23" t="inlineStr">
         <is>
@@ -1690,8 +1734,10 @@
       <c r="G24" t="n">
         <v>2000</v>
       </c>
-      <c r="H24" t="n">
-        <v>40002019</v>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>40002019</t>
+        </is>
       </c>
       <c r="I24" t="inlineStr">
         <is>
@@ -1743,8 +1789,10 @@
       <c r="G25" t="n">
         <v>1000</v>
       </c>
-      <c r="H25" t="n">
-        <v>40002039</v>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>40002039</t>
+        </is>
       </c>
       <c r="I25" t="inlineStr">
         <is>
@@ -1796,8 +1844,10 @@
       <c r="G26" t="n">
         <v>3000</v>
       </c>
-      <c r="H26" t="n">
-        <v>40002047</v>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>40002047</t>
+        </is>
       </c>
       <c r="I26" t="inlineStr">
         <is>
@@ -1849,8 +1899,10 @@
       <c r="G27" t="n">
         <v>1000</v>
       </c>
-      <c r="H27" t="n">
-        <v>40002055</v>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>40002055</t>
+        </is>
       </c>
       <c r="I27" t="inlineStr">
         <is>
@@ -1902,8 +1954,10 @@
       <c r="G28" t="n">
         <v>1750</v>
       </c>
-      <c r="H28" t="n">
-        <v>40002019</v>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>40002019</t>
+        </is>
       </c>
       <c r="I28" t="inlineStr">
         <is>
@@ -1955,8 +2009,10 @@
       <c r="G29" t="n">
         <v>1750</v>
       </c>
-      <c r="H29" t="n">
-        <v>40002019</v>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>40002019</t>
+        </is>
       </c>
       <c r="I29" t="inlineStr">
         <is>
@@ -2008,8 +2064,10 @@
       <c r="G30" t="n">
         <v>500</v>
       </c>
-      <c r="H30" t="n">
-        <v>40002039</v>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>40002039</t>
+        </is>
       </c>
       <c r="I30" t="inlineStr">
         <is>
@@ -2061,8 +2119,10 @@
       <c r="G31" t="n">
         <v>7500</v>
       </c>
-      <c r="H31" t="n">
-        <v>40002019</v>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>40002019</t>
+        </is>
       </c>
       <c r="I31" t="inlineStr">
         <is>
@@ -2114,8 +2174,10 @@
       <c r="G32" t="n">
         <v>1500</v>
       </c>
-      <c r="H32" t="n">
-        <v>40002039</v>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>40002039</t>
+        </is>
       </c>
       <c r="I32" t="inlineStr">
         <is>
@@ -2167,8 +2229,10 @@
       <c r="G33" t="n">
         <v>1500</v>
       </c>
-      <c r="H33" t="n">
-        <v>40002039</v>
+      <c r="H33" t="inlineStr">
+        <is>
+          <t>40002039</t>
+        </is>
       </c>
       <c r="I33" t="inlineStr">
         <is>
@@ -2220,8 +2284,10 @@
       <c r="G34" t="n">
         <v>1500</v>
       </c>
-      <c r="H34" t="n">
-        <v>40002047</v>
+      <c r="H34" t="inlineStr">
+        <is>
+          <t>40002047</t>
+        </is>
       </c>
       <c r="I34" t="inlineStr">
         <is>
@@ -2273,8 +2339,10 @@
       <c r="G35" t="n">
         <v>1000</v>
       </c>
-      <c r="H35" t="n">
-        <v>40002039</v>
+      <c r="H35" t="inlineStr">
+        <is>
+          <t>40002039</t>
+        </is>
       </c>
       <c r="I35" t="inlineStr">
         <is>
@@ -2326,8 +2394,10 @@
       <c r="G36" t="n">
         <v>9000</v>
       </c>
-      <c r="H36" t="n">
-        <v>40002019</v>
+      <c r="H36" t="inlineStr">
+        <is>
+          <t>40002019</t>
+        </is>
       </c>
       <c r="I36" t="inlineStr">
         <is>
@@ -2379,8 +2449,10 @@
       <c r="G37" t="n">
         <v>2000</v>
       </c>
-      <c r="H37" t="n">
-        <v>40002019</v>
+      <c r="H37" t="inlineStr">
+        <is>
+          <t>40002019</t>
+        </is>
       </c>
       <c r="I37" t="inlineStr">
         <is>
@@ -2432,8 +2504,10 @@
       <c r="G38" t="n">
         <v>500</v>
       </c>
-      <c r="H38" t="n">
-        <v>40002039</v>
+      <c r="H38" t="inlineStr">
+        <is>
+          <t>40002039</t>
+        </is>
       </c>
       <c r="I38" t="inlineStr">
         <is>
@@ -2485,8 +2559,10 @@
       <c r="G39" t="n">
         <v>1000</v>
       </c>
-      <c r="H39" t="n">
-        <v>40002047</v>
+      <c r="H39" t="inlineStr">
+        <is>
+          <t>40002047</t>
+        </is>
       </c>
       <c r="I39" t="inlineStr">
         <is>
@@ -2538,8 +2614,10 @@
       <c r="G40" t="n">
         <v>1000</v>
       </c>
-      <c r="H40" t="n">
-        <v>40002055</v>
+      <c r="H40" t="inlineStr">
+        <is>
+          <t>40002055</t>
+        </is>
       </c>
       <c r="I40" t="inlineStr">
         <is>
@@ -2591,8 +2669,10 @@
       <c r="G41" t="n">
         <v>1500</v>
       </c>
-      <c r="H41" t="n">
-        <v>40002039</v>
+      <c r="H41" t="inlineStr">
+        <is>
+          <t>40002039</t>
+        </is>
       </c>
       <c r="I41" t="inlineStr">
         <is>
@@ -2644,8 +2724,10 @@
       <c r="G42" t="n">
         <v>1500</v>
       </c>
-      <c r="H42" t="n">
-        <v>40002047</v>
+      <c r="H42" t="inlineStr">
+        <is>
+          <t>40002047</t>
+        </is>
       </c>
       <c r="I42" t="inlineStr">
         <is>
@@ -2697,8 +2779,10 @@
       <c r="G43" t="n">
         <v>1000</v>
       </c>
-      <c r="H43" t="n">
-        <v>40002055</v>
+      <c r="H43" t="inlineStr">
+        <is>
+          <t>40002055</t>
+        </is>
       </c>
       <c r="I43" t="inlineStr">
         <is>
@@ -2750,8 +2834,10 @@
       <c r="G44" t="n">
         <v>1000</v>
       </c>
-      <c r="H44" t="n">
-        <v>40002039</v>
+      <c r="H44" t="inlineStr">
+        <is>
+          <t>40002039</t>
+        </is>
       </c>
       <c r="I44" t="inlineStr">
         <is>
@@ -2803,8 +2889,10 @@
       <c r="G45" t="n">
         <v>1000</v>
       </c>
-      <c r="H45" t="n">
-        <v>40002047</v>
+      <c r="H45" t="inlineStr">
+        <is>
+          <t>40002047</t>
+        </is>
       </c>
       <c r="I45" t="inlineStr">
         <is>
@@ -2856,8 +2944,10 @@
       <c r="G46" t="n">
         <v>1000</v>
       </c>
-      <c r="H46" t="n">
-        <v>40002055</v>
+      <c r="H46" t="inlineStr">
+        <is>
+          <t>40002055</t>
+        </is>
       </c>
       <c r="I46" t="inlineStr">
         <is>
@@ -2909,8 +2999,10 @@
       <c r="G47" t="n">
         <v>1000</v>
       </c>
-      <c r="H47" t="n">
-        <v>40002039</v>
+      <c r="H47" t="inlineStr">
+        <is>
+          <t>40002039</t>
+        </is>
       </c>
       <c r="I47" t="inlineStr">
         <is>
@@ -2962,8 +3054,10 @@
       <c r="G48" t="n">
         <v>2000</v>
       </c>
-      <c r="H48" t="n">
-        <v>40002047</v>
+      <c r="H48" t="inlineStr">
+        <is>
+          <t>40002047</t>
+        </is>
       </c>
       <c r="I48" t="inlineStr">
         <is>
@@ -3015,8 +3109,10 @@
       <c r="G49" t="n">
         <v>1000</v>
       </c>
-      <c r="H49" t="n">
-        <v>40002055</v>
+      <c r="H49" t="inlineStr">
+        <is>
+          <t>40002055</t>
+        </is>
       </c>
       <c r="I49" t="inlineStr">
         <is>
@@ -3068,8 +3164,10 @@
       <c r="G50" t="n">
         <v>1500</v>
       </c>
-      <c r="H50" t="n">
-        <v>40002019</v>
+      <c r="H50" t="inlineStr">
+        <is>
+          <t>40002019</t>
+        </is>
       </c>
       <c r="I50" t="inlineStr">
         <is>
@@ -3121,8 +3219,10 @@
       <c r="G51" t="n">
         <v>2000</v>
       </c>
-      <c r="H51" t="n">
-        <v>40002039</v>
+      <c r="H51" t="inlineStr">
+        <is>
+          <t>40002039</t>
+        </is>
       </c>
       <c r="I51" t="inlineStr">
         <is>
@@ -3174,8 +3274,10 @@
       <c r="G52" t="n">
         <v>2000</v>
       </c>
-      <c r="H52" t="n">
-        <v>40002047</v>
+      <c r="H52" t="inlineStr">
+        <is>
+          <t>40002047</t>
+        </is>
       </c>
       <c r="I52" t="inlineStr">
         <is>
@@ -3227,8 +3329,10 @@
       <c r="G53" t="n">
         <v>2000</v>
       </c>
-      <c r="H53" t="n">
-        <v>40002055</v>
+      <c r="H53" t="inlineStr">
+        <is>
+          <t>40002055</t>
+        </is>
       </c>
       <c r="I53" t="inlineStr">
         <is>
@@ -3280,8 +3384,10 @@
       <c r="G54" t="n">
         <v>3000</v>
       </c>
-      <c r="H54" t="n">
-        <v>40002019</v>
+      <c r="H54" t="inlineStr">
+        <is>
+          <t>40002019</t>
+        </is>
       </c>
       <c r="I54" t="inlineStr">
         <is>
@@ -3333,8 +3439,10 @@
       <c r="G55" t="n">
         <v>1000</v>
       </c>
-      <c r="H55" t="n">
-        <v>40002039</v>
+      <c r="H55" t="inlineStr">
+        <is>
+          <t>40002039</t>
+        </is>
       </c>
       <c r="I55" t="inlineStr">
         <is>
@@ -3386,8 +3494,10 @@
       <c r="G56" t="n">
         <v>1500</v>
       </c>
-      <c r="H56" t="n">
-        <v>40002047</v>
+      <c r="H56" t="inlineStr">
+        <is>
+          <t>40002047</t>
+        </is>
       </c>
       <c r="I56" t="inlineStr">
         <is>
@@ -3439,8 +3549,10 @@
       <c r="G57" t="n">
         <v>500</v>
       </c>
-      <c r="H57" t="n">
-        <v>40002055</v>
+      <c r="H57" t="inlineStr">
+        <is>
+          <t>40002055</t>
+        </is>
       </c>
       <c r="I57" t="inlineStr">
         <is>
@@ -3492,8 +3604,10 @@
       <c r="G58" t="n">
         <v>7500</v>
       </c>
-      <c r="H58" t="n">
-        <v>40002019</v>
+      <c r="H58" t="inlineStr">
+        <is>
+          <t>40002019</t>
+        </is>
       </c>
       <c r="I58" t="inlineStr">
         <is>
@@ -3545,8 +3659,10 @@
       <c r="G59" t="n">
         <v>6500</v>
       </c>
-      <c r="H59" t="n">
-        <v>40002019</v>
+      <c r="H59" t="inlineStr">
+        <is>
+          <t>40002019</t>
+        </is>
       </c>
       <c r="I59" t="inlineStr">
         <is>
@@ -3598,8 +3714,10 @@
       <c r="G60" t="n">
         <v>1500</v>
       </c>
-      <c r="H60" t="n">
-        <v>40002039</v>
+      <c r="H60" t="inlineStr">
+        <is>
+          <t>40002039</t>
+        </is>
       </c>
       <c r="I60" t="inlineStr">
         <is>
@@ -3651,8 +3769,10 @@
       <c r="G61" t="n">
         <v>1000</v>
       </c>
-      <c r="H61" t="n">
-        <v>40002047</v>
+      <c r="H61" t="inlineStr">
+        <is>
+          <t>40002047</t>
+        </is>
       </c>
       <c r="I61" t="inlineStr">
         <is>
@@ -3704,8 +3824,10 @@
       <c r="G62" t="n">
         <v>1000</v>
       </c>
-      <c r="H62" t="n">
-        <v>40002019</v>
+      <c r="H62" t="inlineStr">
+        <is>
+          <t>40002019</t>
+        </is>
       </c>
       <c r="I62" t="inlineStr">
         <is>
@@ -3757,8 +3879,10 @@
       <c r="G63" t="n">
         <v>3000</v>
       </c>
-      <c r="H63" t="n">
-        <v>40002039</v>
+      <c r="H63" t="inlineStr">
+        <is>
+          <t>40002039</t>
+        </is>
       </c>
       <c r="I63" t="inlineStr">
         <is>
@@ -3810,8 +3934,10 @@
       <c r="G64" t="n">
         <v>3500</v>
       </c>
-      <c r="H64" t="n">
-        <v>40002047</v>
+      <c r="H64" t="inlineStr">
+        <is>
+          <t>40002047</t>
+        </is>
       </c>
       <c r="I64" t="inlineStr">
         <is>
@@ -3863,8 +3989,10 @@
       <c r="G65" t="n">
         <v>1500</v>
       </c>
-      <c r="H65" t="n">
-        <v>40002055</v>
+      <c r="H65" t="inlineStr">
+        <is>
+          <t>40002055</t>
+        </is>
       </c>
       <c r="I65" t="inlineStr">
         <is>
@@ -3916,8 +4044,10 @@
       <c r="G66" t="n">
         <v>1500</v>
       </c>
-      <c r="H66" t="n">
-        <v>40002019</v>
+      <c r="H66" t="inlineStr">
+        <is>
+          <t>40002019</t>
+        </is>
       </c>
       <c r="I66" t="inlineStr">
         <is>
@@ -3969,8 +4099,10 @@
       <c r="G67" t="n">
         <v>2000</v>
       </c>
-      <c r="H67" t="n">
-        <v>40002039</v>
+      <c r="H67" t="inlineStr">
+        <is>
+          <t>40002039</t>
+        </is>
       </c>
       <c r="I67" t="inlineStr">
         <is>
@@ -4022,8 +4154,10 @@
       <c r="G68" t="n">
         <v>500</v>
       </c>
-      <c r="H68" t="n">
-        <v>40002047</v>
+      <c r="H68" t="inlineStr">
+        <is>
+          <t>40002047</t>
+        </is>
       </c>
       <c r="I68" t="inlineStr">
         <is>
@@ -4075,8 +4209,10 @@
       <c r="G69" t="n">
         <v>2000</v>
       </c>
-      <c r="H69" t="n">
-        <v>40002023</v>
+      <c r="H69" t="inlineStr">
+        <is>
+          <t>40002023</t>
+        </is>
       </c>
       <c r="I69" t="inlineStr">
         <is>
@@ -4128,8 +4264,10 @@
       <c r="G70" t="n">
         <v>1000</v>
       </c>
-      <c r="H70" t="n">
-        <v>40002041</v>
+      <c r="H70" t="inlineStr">
+        <is>
+          <t>40002041</t>
+        </is>
       </c>
       <c r="I70" t="inlineStr">
         <is>
@@ -4181,8 +4319,10 @@
       <c r="G71" t="n">
         <v>1000</v>
       </c>
-      <c r="H71" t="n">
-        <v>40002049</v>
+      <c r="H71" t="inlineStr">
+        <is>
+          <t>40002049</t>
+        </is>
       </c>
       <c r="I71" t="inlineStr">
         <is>
@@ -4234,8 +4374,10 @@
       <c r="G72" t="n">
         <v>3000</v>
       </c>
-      <c r="H72" t="n">
-        <v>40002019</v>
+      <c r="H72" t="inlineStr">
+        <is>
+          <t>40002019</t>
+        </is>
       </c>
       <c r="I72" t="inlineStr">
         <is>
@@ -4287,8 +4429,10 @@
       <c r="G73" t="n">
         <v>6000</v>
       </c>
-      <c r="H73" t="n">
-        <v>40002019</v>
+      <c r="H73" t="inlineStr">
+        <is>
+          <t>40002019</t>
+        </is>
       </c>
       <c r="I73" t="inlineStr">
         <is>
@@ -4340,8 +4484,10 @@
       <c r="G74" t="n">
         <v>500</v>
       </c>
-      <c r="H74" t="n">
-        <v>40002019</v>
+      <c r="H74" t="inlineStr">
+        <is>
+          <t>40002019</t>
+        </is>
       </c>
       <c r="I74" t="inlineStr">
         <is>
@@ -4393,8 +4539,10 @@
       <c r="G75" t="n">
         <v>1000</v>
       </c>
-      <c r="H75" t="n">
-        <v>40002039</v>
+      <c r="H75" t="inlineStr">
+        <is>
+          <t>40002039</t>
+        </is>
       </c>
       <c r="I75" t="inlineStr">
         <is>
@@ -4446,8 +4594,10 @@
       <c r="G76" t="n">
         <v>1500</v>
       </c>
-      <c r="H76" t="n">
-        <v>40002047</v>
+      <c r="H76" t="inlineStr">
+        <is>
+          <t>40002047</t>
+        </is>
       </c>
       <c r="I76" t="inlineStr">
         <is>
@@ -4499,8 +4649,10 @@
       <c r="G77" t="n">
         <v>2000</v>
       </c>
-      <c r="H77" t="n">
-        <v>40002019</v>
+      <c r="H77" t="inlineStr">
+        <is>
+          <t>40002019</t>
+        </is>
       </c>
       <c r="I77" t="inlineStr">
         <is>
@@ -4552,8 +4704,10 @@
       <c r="G78" t="n">
         <v>1000</v>
       </c>
-      <c r="H78" t="n">
-        <v>40002019</v>
+      <c r="H78" t="inlineStr">
+        <is>
+          <t>40002019</t>
+        </is>
       </c>
       <c r="I78" t="inlineStr">
         <is>
@@ -4605,8 +4759,10 @@
       <c r="G79" t="n">
         <v>1000</v>
       </c>
-      <c r="H79" t="n">
-        <v>40002039</v>
+      <c r="H79" t="inlineStr">
+        <is>
+          <t>40002039</t>
+        </is>
       </c>
       <c r="I79" t="inlineStr">
         <is>
@@ -4658,8 +4814,10 @@
       <c r="G80" t="n">
         <v>1000</v>
       </c>
-      <c r="H80" t="n">
-        <v>40002047</v>
+      <c r="H80" t="inlineStr">
+        <is>
+          <t>40002047</t>
+        </is>
       </c>
       <c r="I80" t="inlineStr">
         <is>
@@ -4711,8 +4869,10 @@
       <c r="G81" t="n">
         <v>1000</v>
       </c>
-      <c r="H81" t="n">
-        <v>40002019</v>
+      <c r="H81" t="inlineStr">
+        <is>
+          <t>40002019</t>
+        </is>
       </c>
       <c r="I81" t="inlineStr">
         <is>
@@ -4764,8 +4924,10 @@
       <c r="G82" t="n">
         <v>2500</v>
       </c>
-      <c r="H82" t="n">
-        <v>40002019</v>
+      <c r="H82" t="inlineStr">
+        <is>
+          <t>40002019</t>
+        </is>
       </c>
       <c r="I82" t="inlineStr">
         <is>
@@ -4817,8 +4979,10 @@
       <c r="G83" t="n">
         <v>1000</v>
       </c>
-      <c r="H83" t="n">
-        <v>40002039</v>
+      <c r="H83" t="inlineStr">
+        <is>
+          <t>40002039</t>
+        </is>
       </c>
       <c r="I83" t="inlineStr">
         <is>
@@ -4870,8 +5034,10 @@
       <c r="G84" t="n">
         <v>500</v>
       </c>
-      <c r="H84" t="n">
-        <v>40002047</v>
+      <c r="H84" t="inlineStr">
+        <is>
+          <t>40002047</t>
+        </is>
       </c>
       <c r="I84" t="inlineStr">
         <is>
@@ -4923,8 +5089,10 @@
       <c r="G85" t="n">
         <v>2000</v>
       </c>
-      <c r="H85" t="n">
-        <v>40002019</v>
+      <c r="H85" t="inlineStr">
+        <is>
+          <t>40002019</t>
+        </is>
       </c>
       <c r="I85" t="inlineStr">
         <is>
@@ -4976,8 +5144,10 @@
       <c r="G86" t="n">
         <v>1000</v>
       </c>
-      <c r="H86" t="n">
-        <v>40002039</v>
+      <c r="H86" t="inlineStr">
+        <is>
+          <t>40002039</t>
+        </is>
       </c>
       <c r="I86" t="inlineStr">
         <is>
@@ -5029,8 +5199,10 @@
       <c r="G87" t="n">
         <v>500</v>
       </c>
-      <c r="H87" t="n">
-        <v>40002047</v>
+      <c r="H87" t="inlineStr">
+        <is>
+          <t>40002047</t>
+        </is>
       </c>
       <c r="I87" t="inlineStr">
         <is>
@@ -5082,8 +5254,10 @@
       <c r="G88" t="n">
         <v>500</v>
       </c>
-      <c r="H88" t="n">
-        <v>40002055</v>
+      <c r="H88" t="inlineStr">
+        <is>
+          <t>40002055</t>
+        </is>
       </c>
       <c r="I88" t="inlineStr">
         <is>
@@ -5135,8 +5309,10 @@
       <c r="G89" t="n">
         <v>2000</v>
       </c>
-      <c r="H89" t="n">
-        <v>40002023</v>
+      <c r="H89" t="inlineStr">
+        <is>
+          <t>40002023</t>
+        </is>
       </c>
       <c r="I89" t="inlineStr">
         <is>
@@ -5188,8 +5364,10 @@
       <c r="G90" t="n">
         <v>1000</v>
       </c>
-      <c r="H90" t="n">
-        <v>40002041</v>
+      <c r="H90" t="inlineStr">
+        <is>
+          <t>40002041</t>
+        </is>
       </c>
       <c r="I90" t="inlineStr">
         <is>
@@ -5241,8 +5419,10 @@
       <c r="G91" t="n">
         <v>500</v>
       </c>
-      <c r="H91" t="n">
-        <v>40002049</v>
+      <c r="H91" t="inlineStr">
+        <is>
+          <t>40002049</t>
+        </is>
       </c>
       <c r="I91" t="inlineStr">
         <is>
@@ -5294,8 +5474,10 @@
       <c r="G92" t="n">
         <v>500</v>
       </c>
-      <c r="H92" t="n">
-        <v>40002057</v>
+      <c r="H92" t="inlineStr">
+        <is>
+          <t>40002057</t>
+        </is>
       </c>
       <c r="I92" t="inlineStr">
         <is>
@@ -5347,8 +5529,10 @@
       <c r="G93" t="n">
         <v>500</v>
       </c>
-      <c r="H93" t="n">
-        <v>40002019</v>
+      <c r="H93" t="inlineStr">
+        <is>
+          <t>40002019</t>
+        </is>
       </c>
       <c r="I93" t="inlineStr">
         <is>
@@ -5400,8 +5584,10 @@
       <c r="G94" t="n">
         <v>1000</v>
       </c>
-      <c r="H94" t="n">
-        <v>40002039</v>
+      <c r="H94" t="inlineStr">
+        <is>
+          <t>40002039</t>
+        </is>
       </c>
       <c r="I94" t="inlineStr">
         <is>
@@ -5453,8 +5639,10 @@
       <c r="G95" t="n">
         <v>2000</v>
       </c>
-      <c r="H95" t="n">
-        <v>40002047</v>
+      <c r="H95" t="inlineStr">
+        <is>
+          <t>40002047</t>
+        </is>
       </c>
       <c r="I95" t="inlineStr">
         <is>
@@ -5506,8 +5694,10 @@
       <c r="G96" t="n">
         <v>500</v>
       </c>
-      <c r="H96" t="n">
-        <v>40002055</v>
+      <c r="H96" t="inlineStr">
+        <is>
+          <t>40002055</t>
+        </is>
       </c>
       <c r="I96" t="inlineStr">
         <is>
@@ -5559,8 +5749,10 @@
       <c r="G97" t="n">
         <v>500</v>
       </c>
-      <c r="H97" t="n">
-        <v>40002019</v>
+      <c r="H97" t="inlineStr">
+        <is>
+          <t>40002019</t>
+        </is>
       </c>
       <c r="I97" t="inlineStr">
         <is>
@@ -5612,8 +5804,10 @@
       <c r="G98" t="n">
         <v>1000</v>
       </c>
-      <c r="H98" t="n">
-        <v>40002039</v>
+      <c r="H98" t="inlineStr">
+        <is>
+          <t>40002039</t>
+        </is>
       </c>
       <c r="I98" t="inlineStr">
         <is>
@@ -5665,8 +5859,10 @@
       <c r="G99" t="n">
         <v>1500</v>
       </c>
-      <c r="H99" t="n">
-        <v>40002047</v>
+      <c r="H99" t="inlineStr">
+        <is>
+          <t>40002047</t>
+        </is>
       </c>
       <c r="I99" t="inlineStr">
         <is>
@@ -5718,8 +5914,10 @@
       <c r="G100" t="n">
         <v>1000</v>
       </c>
-      <c r="H100" t="n">
-        <v>40002055</v>
+      <c r="H100" t="inlineStr">
+        <is>
+          <t>40002055</t>
+        </is>
       </c>
       <c r="I100" t="inlineStr">
         <is>
@@ -5771,8 +5969,10 @@
       <c r="G101" t="n">
         <v>1500</v>
       </c>
-      <c r="H101" t="n">
-        <v>40002055</v>
+      <c r="H101" t="inlineStr">
+        <is>
+          <t>40002055</t>
+        </is>
       </c>
       <c r="I101" t="inlineStr">
         <is>
@@ -5824,8 +6024,10 @@
       <c r="G102" t="n">
         <v>1000</v>
       </c>
-      <c r="H102" t="n">
-        <v>40002019</v>
+      <c r="H102" t="inlineStr">
+        <is>
+          <t>40002019</t>
+        </is>
       </c>
       <c r="I102" t="inlineStr">
         <is>
@@ -5877,8 +6079,10 @@
       <c r="G103" t="n">
         <v>500</v>
       </c>
-      <c r="H103" t="n">
-        <v>40002039</v>
+      <c r="H103" t="inlineStr">
+        <is>
+          <t>40002039</t>
+        </is>
       </c>
       <c r="I103" t="inlineStr">
         <is>
@@ -5930,8 +6134,10 @@
       <c r="G104" t="n">
         <v>500</v>
       </c>
-      <c r="H104" t="n">
-        <v>40002055</v>
+      <c r="H104" t="inlineStr">
+        <is>
+          <t>40002055</t>
+        </is>
       </c>
       <c r="I104" t="inlineStr">
         <is>
@@ -5983,8 +6189,10 @@
       <c r="G105" t="n">
         <v>2000</v>
       </c>
-      <c r="H105" t="n">
-        <v>40002047</v>
+      <c r="H105" t="inlineStr">
+        <is>
+          <t>40002047</t>
+        </is>
       </c>
       <c r="I105" t="inlineStr">
         <is>
@@ -6036,8 +6244,10 @@
       <c r="G106" t="n">
         <v>500</v>
       </c>
-      <c r="H106" t="n">
-        <v>40002055</v>
+      <c r="H106" t="inlineStr">
+        <is>
+          <t>40002055</t>
+        </is>
       </c>
       <c r="I106" t="inlineStr">
         <is>
@@ -6089,8 +6299,10 @@
       <c r="G107" t="n">
         <v>1000</v>
       </c>
-      <c r="H107" t="n">
-        <v>40002039</v>
+      <c r="H107" t="inlineStr">
+        <is>
+          <t>40002039</t>
+        </is>
       </c>
       <c r="I107" t="inlineStr">
         <is>
@@ -6142,8 +6354,10 @@
       <c r="G108" t="n">
         <v>2500</v>
       </c>
-      <c r="H108" t="n">
-        <v>40002047</v>
+      <c r="H108" t="inlineStr">
+        <is>
+          <t>40002047</t>
+        </is>
       </c>
       <c r="I108" t="inlineStr">
         <is>
@@ -6195,8 +6409,10 @@
       <c r="G109" t="n">
         <v>1000</v>
       </c>
-      <c r="H109" t="n">
-        <v>40002055</v>
+      <c r="H109" t="inlineStr">
+        <is>
+          <t>40002055</t>
+        </is>
       </c>
       <c r="I109" t="inlineStr">
         <is>
@@ -6248,8 +6464,10 @@
       <c r="G110" t="n">
         <v>2000</v>
       </c>
-      <c r="H110" t="n">
-        <v>40002019</v>
+      <c r="H110" t="inlineStr">
+        <is>
+          <t>40002019</t>
+        </is>
       </c>
       <c r="I110" t="inlineStr">
         <is>
@@ -6301,8 +6519,10 @@
       <c r="G111" t="n">
         <v>3250</v>
       </c>
-      <c r="H111" t="n">
-        <v>40002039</v>
+      <c r="H111" t="inlineStr">
+        <is>
+          <t>40002039</t>
+        </is>
       </c>
       <c r="I111" t="inlineStr">
         <is>
@@ -6354,8 +6574,10 @@
       <c r="G112" t="n">
         <v>750</v>
       </c>
-      <c r="H112" t="n">
-        <v>40002047</v>
+      <c r="H112" t="inlineStr">
+        <is>
+          <t>40002047</t>
+        </is>
       </c>
       <c r="I112" t="inlineStr">
         <is>
@@ -6407,8 +6629,10 @@
       <c r="G113" t="n">
         <v>3000</v>
       </c>
-      <c r="H113" t="n">
-        <v>40002019</v>
+      <c r="H113" t="inlineStr">
+        <is>
+          <t>40002019</t>
+        </is>
       </c>
       <c r="I113" t="inlineStr">
         <is>
@@ -6460,8 +6684,10 @@
       <c r="G114" t="n">
         <v>1000</v>
       </c>
-      <c r="H114" t="n">
-        <v>40002039</v>
+      <c r="H114" t="inlineStr">
+        <is>
+          <t>40002039</t>
+        </is>
       </c>
       <c r="I114" t="inlineStr">
         <is>
@@ -6513,8 +6739,10 @@
       <c r="G115" t="n">
         <v>1000</v>
       </c>
-      <c r="H115" t="n">
-        <v>40002047</v>
+      <c r="H115" t="inlineStr">
+        <is>
+          <t>40002047</t>
+        </is>
       </c>
       <c r="I115" t="inlineStr">
         <is>
@@ -6566,8 +6794,10 @@
       <c r="G116" t="n">
         <v>1000</v>
       </c>
-      <c r="H116" t="n">
-        <v>40002019</v>
+      <c r="H116" t="inlineStr">
+        <is>
+          <t>40002019</t>
+        </is>
       </c>
       <c r="I116" t="inlineStr">
         <is>
@@ -6619,8 +6849,10 @@
       <c r="G117" t="n">
         <v>1000</v>
       </c>
-      <c r="H117" t="n">
-        <v>40002039</v>
+      <c r="H117" t="inlineStr">
+        <is>
+          <t>40002039</t>
+        </is>
       </c>
       <c r="I117" t="inlineStr">
         <is>
@@ -6672,8 +6904,10 @@
       <c r="G118" t="n">
         <v>1500</v>
       </c>
-      <c r="H118" t="n">
-        <v>40002047</v>
+      <c r="H118" t="inlineStr">
+        <is>
+          <t>40002047</t>
+        </is>
       </c>
       <c r="I118" t="inlineStr">
         <is>
@@ -6725,8 +6959,10 @@
       <c r="G119" t="n">
         <v>500</v>
       </c>
-      <c r="H119" t="n">
-        <v>40002055</v>
+      <c r="H119" t="inlineStr">
+        <is>
+          <t>40002055</t>
+        </is>
       </c>
       <c r="I119" t="inlineStr">
         <is>
@@ -6778,8 +7014,10 @@
       <c r="G120" t="n">
         <v>2000</v>
       </c>
-      <c r="H120" t="n">
-        <v>40002019</v>
+      <c r="H120" t="inlineStr">
+        <is>
+          <t>40002019</t>
+        </is>
       </c>
       <c r="I120" t="inlineStr">
         <is>
@@ -6831,8 +7069,10 @@
       <c r="G121" t="n">
         <v>500</v>
       </c>
-      <c r="H121" t="n">
-        <v>40002039</v>
+      <c r="H121" t="inlineStr">
+        <is>
+          <t>40002039</t>
+        </is>
       </c>
       <c r="I121" t="inlineStr">
         <is>
@@ -6884,8 +7124,10 @@
       <c r="G122" t="n">
         <v>8000</v>
       </c>
-      <c r="H122" t="n">
-        <v>40002019</v>
+      <c r="H122" t="inlineStr">
+        <is>
+          <t>40002019</t>
+        </is>
       </c>
       <c r="I122" t="inlineStr">
         <is>
@@ -6937,8 +7179,10 @@
       <c r="G123" t="n">
         <v>500</v>
       </c>
-      <c r="H123" t="n">
-        <v>40002047</v>
+      <c r="H123" t="inlineStr">
+        <is>
+          <t>40002047</t>
+        </is>
       </c>
       <c r="I123" t="inlineStr">
         <is>
@@ -6990,8 +7234,10 @@
       <c r="G124" t="n">
         <v>3000</v>
       </c>
-      <c r="H124" t="n">
-        <v>40002019</v>
+      <c r="H124" t="inlineStr">
+        <is>
+          <t>40002019</t>
+        </is>
       </c>
       <c r="I124" t="inlineStr">
         <is>
@@ -7043,8 +7289,10 @@
       <c r="G125" t="n">
         <v>1000</v>
       </c>
-      <c r="H125" t="n">
-        <v>40002039</v>
+      <c r="H125" t="inlineStr">
+        <is>
+          <t>40002039</t>
+        </is>
       </c>
       <c r="I125" t="inlineStr">
         <is>
@@ -7096,8 +7344,10 @@
       <c r="G126" t="n">
         <v>500</v>
       </c>
-      <c r="H126" t="n">
-        <v>40002019</v>
+      <c r="H126" t="inlineStr">
+        <is>
+          <t>40002019</t>
+        </is>
       </c>
       <c r="I126" t="inlineStr">
         <is>
@@ -7149,8 +7399,10 @@
       <c r="G127" t="n">
         <v>1000</v>
       </c>
-      <c r="H127" t="n">
-        <v>40002039</v>
+      <c r="H127" t="inlineStr">
+        <is>
+          <t>40002039</t>
+        </is>
       </c>
       <c r="I127" t="inlineStr">
         <is>
@@ -7202,8 +7454,10 @@
       <c r="G128" t="n">
         <v>2000</v>
       </c>
-      <c r="H128" t="n">
-        <v>40002047</v>
+      <c r="H128" t="inlineStr">
+        <is>
+          <t>40002047</t>
+        </is>
       </c>
       <c r="I128" t="inlineStr">
         <is>
@@ -7255,8 +7509,10 @@
       <c r="G129" t="n">
         <v>500</v>
       </c>
-      <c r="H129" t="n">
-        <v>40002055</v>
+      <c r="H129" t="inlineStr">
+        <is>
+          <t>40002055</t>
+        </is>
       </c>
       <c r="I129" t="inlineStr">
         <is>
@@ -7308,8 +7564,10 @@
       <c r="G130" t="n">
         <v>1000</v>
       </c>
-      <c r="H130" t="n">
-        <v>40002039</v>
+      <c r="H130" t="inlineStr">
+        <is>
+          <t>40002039</t>
+        </is>
       </c>
       <c r="I130" t="inlineStr">
         <is>
@@ -7361,8 +7619,10 @@
       <c r="G131" t="n">
         <v>2000</v>
       </c>
-      <c r="H131" t="n">
-        <v>40002047</v>
+      <c r="H131" t="inlineStr">
+        <is>
+          <t>40002047</t>
+        </is>
       </c>
       <c r="I131" t="inlineStr">
         <is>
@@ -7414,8 +7674,10 @@
       <c r="G132" t="n">
         <v>1000</v>
       </c>
-      <c r="H132" t="n">
-        <v>40002055</v>
+      <c r="H132" t="inlineStr">
+        <is>
+          <t>40002055</t>
+        </is>
       </c>
       <c r="I132" t="inlineStr">
         <is>
@@ -7467,8 +7729,10 @@
       <c r="G133" t="n">
         <v>500</v>
       </c>
-      <c r="H133" t="n">
-        <v>40002019</v>
+      <c r="H133" t="inlineStr">
+        <is>
+          <t>40002019</t>
+        </is>
       </c>
       <c r="I133" t="inlineStr">
         <is>
@@ -7520,8 +7784,10 @@
       <c r="G134" t="n">
         <v>2000</v>
       </c>
-      <c r="H134" t="n">
-        <v>40002039</v>
+      <c r="H134" t="inlineStr">
+        <is>
+          <t>40002039</t>
+        </is>
       </c>
       <c r="I134" t="inlineStr">
         <is>
@@ -7573,8 +7839,10 @@
       <c r="G135" t="n">
         <v>2500</v>
       </c>
-      <c r="H135" t="n">
-        <v>40002047</v>
+      <c r="H135" t="inlineStr">
+        <is>
+          <t>40002047</t>
+        </is>
       </c>
       <c r="I135" t="inlineStr">
         <is>
@@ -7626,8 +7894,10 @@
       <c r="G136" t="n">
         <v>1000</v>
       </c>
-      <c r="H136" t="n">
-        <v>40002055</v>
+      <c r="H136" t="inlineStr">
+        <is>
+          <t>40002055</t>
+        </is>
       </c>
       <c r="I136" t="inlineStr">
         <is>
@@ -7679,8 +7949,10 @@
       <c r="G137" t="n">
         <v>3000</v>
       </c>
-      <c r="H137" t="n">
-        <v>40002019</v>
+      <c r="H137" t="inlineStr">
+        <is>
+          <t>40002019</t>
+        </is>
       </c>
       <c r="I137" t="inlineStr">
         <is>
@@ -7732,8 +8004,10 @@
       <c r="G138" t="n">
         <v>500</v>
       </c>
-      <c r="H138" t="n">
-        <v>40002039</v>
+      <c r="H138" t="inlineStr">
+        <is>
+          <t>40002039</t>
+        </is>
       </c>
       <c r="I138" t="inlineStr">
         <is>
@@ -7785,8 +8059,10 @@
       <c r="G139" t="n">
         <v>500</v>
       </c>
-      <c r="H139" t="n">
-        <v>40002047</v>
+      <c r="H139" t="inlineStr">
+        <is>
+          <t>40002047</t>
+        </is>
       </c>
       <c r="I139" t="inlineStr">
         <is>
@@ -7838,8 +8114,10 @@
       <c r="G140" t="n">
         <v>2000</v>
       </c>
-      <c r="H140" t="n">
-        <v>40002019</v>
+      <c r="H140" t="inlineStr">
+        <is>
+          <t>40002019</t>
+        </is>
       </c>
       <c r="I140" t="inlineStr">
         <is>
@@ -7891,8 +8169,10 @@
       <c r="G141" t="n">
         <v>1000</v>
       </c>
-      <c r="H141" t="n">
-        <v>40002039</v>
+      <c r="H141" t="inlineStr">
+        <is>
+          <t>40002039</t>
+        </is>
       </c>
       <c r="I141" t="inlineStr">
         <is>
@@ -7944,8 +8224,10 @@
       <c r="G142" t="n">
         <v>1000</v>
       </c>
-      <c r="H142" t="n">
-        <v>40002047</v>
+      <c r="H142" t="inlineStr">
+        <is>
+          <t>40002047</t>
+        </is>
       </c>
       <c r="I142" t="inlineStr">
         <is>
@@ -7997,8 +8279,10 @@
       <c r="G143" t="n">
         <v>500</v>
       </c>
-      <c r="H143" t="n">
-        <v>40002039</v>
+      <c r="H143" t="inlineStr">
+        <is>
+          <t>40002039</t>
+        </is>
       </c>
       <c r="I143" t="inlineStr">
         <is>
@@ -8050,8 +8334,10 @@
       <c r="G144" t="n">
         <v>500</v>
       </c>
-      <c r="H144" t="n">
-        <v>40002039</v>
+      <c r="H144" t="inlineStr">
+        <is>
+          <t>40002039</t>
+        </is>
       </c>
       <c r="I144" t="inlineStr">
         <is>
@@ -8103,8 +8389,10 @@
       <c r="G145" t="n">
         <v>1500</v>
       </c>
-      <c r="H145" t="n">
-        <v>40002019</v>
+      <c r="H145" t="inlineStr">
+        <is>
+          <t>40002019</t>
+        </is>
       </c>
       <c r="I145" t="inlineStr">
         <is>
@@ -8156,8 +8444,10 @@
       <c r="G146" t="n">
         <v>1000</v>
       </c>
-      <c r="H146" t="n">
-        <v>40002047</v>
+      <c r="H146" t="inlineStr">
+        <is>
+          <t>40002047</t>
+        </is>
       </c>
       <c r="I146" t="inlineStr">
         <is>
@@ -8209,8 +8499,10 @@
       <c r="G147" t="n">
         <v>500</v>
       </c>
-      <c r="H147" t="n">
-        <v>40002055</v>
+      <c r="H147" t="inlineStr">
+        <is>
+          <t>40002055</t>
+        </is>
       </c>
       <c r="I147" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Se agregan los terminales al mapa
</commit_message>
<xml_diff>
--- a/datos_intermedios/Data_Filtrada_COESTI.xlsx
+++ b/datos_intermedios/Data_Filtrada_COESTI.xlsx
@@ -541,7 +541,7 @@
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>Terminal PBF Callao</t>
+          <t>TERMINAL PBF CALLAO</t>
         </is>
       </c>
     </row>
@@ -596,7 +596,7 @@
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>Terminal Refinería Pampilla</t>
+          <t>TERMINAL REFINERÍA PAMPILLA</t>
         </is>
       </c>
     </row>
@@ -651,7 +651,7 @@
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>Terminal Refinería Pampilla</t>
+          <t>TERMINAL REFINERÍA PAMPILLA</t>
         </is>
       </c>
     </row>
@@ -706,7 +706,7 @@
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>Terminal Refinería Pampilla</t>
+          <t>TERMINAL REFINERÍA PAMPILLA</t>
         </is>
       </c>
     </row>
@@ -761,7 +761,7 @@
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>Terminal Refinería Pampilla</t>
+          <t>TERMINAL REFINERÍA PAMPILLA</t>
         </is>
       </c>
     </row>
@@ -816,7 +816,7 @@
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>Terminal Refinería Pampilla</t>
+          <t>TERMINAL REFINERÍA PAMPILLA</t>
         </is>
       </c>
     </row>
@@ -871,7 +871,7 @@
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>Terminal Refinería Pampilla</t>
+          <t>TERMINAL REFINERÍA PAMPILLA</t>
         </is>
       </c>
     </row>
@@ -926,7 +926,7 @@
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>Terminal Refinería Pampilla</t>
+          <t>TERMINAL REFINERÍA PAMPILLA</t>
         </is>
       </c>
     </row>
@@ -981,7 +981,7 @@
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>Terminal Refinería Conchán</t>
+          <t>TERMINAL REFINERÍA CONCHÁN</t>
         </is>
       </c>
     </row>
@@ -1036,7 +1036,7 @@
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>Terminal Refinería Conchán</t>
+          <t>TERMINAL REFINERÍA CONCHÁN</t>
         </is>
       </c>
     </row>
@@ -1091,7 +1091,7 @@
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>Terminal Refinería Conchán</t>
+          <t>TERMINAL REFINERÍA CONCHÁN</t>
         </is>
       </c>
     </row>
@@ -1146,7 +1146,7 @@
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>Terminal PBF Callao</t>
+          <t>TERMINAL PBF CALLAO</t>
         </is>
       </c>
     </row>
@@ -1201,7 +1201,7 @@
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>Terminal PBF Callao</t>
+          <t>TERMINAL PBF CALLAO</t>
         </is>
       </c>
     </row>
@@ -1256,7 +1256,7 @@
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>Terminal PBF Callao</t>
+          <t>TERMINAL PBF CALLAO</t>
         </is>
       </c>
     </row>
@@ -1311,7 +1311,7 @@
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>Terminal PBF Callao</t>
+          <t>TERMINAL PBF CALLAO</t>
         </is>
       </c>
     </row>
@@ -1366,7 +1366,7 @@
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>Terminal PBF Callao</t>
+          <t>TERMINAL PBF CALLAO</t>
         </is>
       </c>
     </row>
@@ -1421,7 +1421,7 @@
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>Terminal PBF Callao</t>
+          <t>TERMINAL PBF CALLAO</t>
         </is>
       </c>
     </row>
@@ -1476,7 +1476,7 @@
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>Terminal PBF Callao</t>
+          <t>TERMINAL PBF CALLAO</t>
         </is>
       </c>
     </row>
@@ -1531,7 +1531,7 @@
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>Terminal PBF Callao</t>
+          <t>TERMINAL PBF CALLAO</t>
         </is>
       </c>
     </row>
@@ -1586,7 +1586,7 @@
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>Terminal PBF Callao</t>
+          <t>TERMINAL PBF CALLAO</t>
         </is>
       </c>
     </row>
@@ -1641,7 +1641,7 @@
       </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>Terminal PBF Callao</t>
+          <t>TERMINAL PBF CALLAO</t>
         </is>
       </c>
     </row>
@@ -1696,7 +1696,7 @@
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>Terminal Refinería Conchán</t>
+          <t>TERMINAL REFINERÍA CONCHÁN</t>
         </is>
       </c>
     </row>
@@ -1751,7 +1751,7 @@
       </c>
       <c r="K24" t="inlineStr">
         <is>
-          <t>Terminal Refinería Conchán</t>
+          <t>TERMINAL REFINERÍA CONCHÁN</t>
         </is>
       </c>
     </row>
@@ -1806,7 +1806,7 @@
       </c>
       <c r="K25" t="inlineStr">
         <is>
-          <t>Terminal Refinería Conchán</t>
+          <t>TERMINAL REFINERÍA CONCHÁN</t>
         </is>
       </c>
     </row>
@@ -1861,7 +1861,7 @@
       </c>
       <c r="K26" t="inlineStr">
         <is>
-          <t>Terminal Refinería Conchán</t>
+          <t>TERMINAL REFINERÍA CONCHÁN</t>
         </is>
       </c>
     </row>
@@ -1916,7 +1916,7 @@
       </c>
       <c r="K27" t="inlineStr">
         <is>
-          <t>Terminal Refinería Conchán</t>
+          <t>TERMINAL REFINERÍA CONCHÁN</t>
         </is>
       </c>
     </row>
@@ -1971,7 +1971,7 @@
       </c>
       <c r="K28" t="inlineStr">
         <is>
-          <t>Terminal Refinería Pampilla</t>
+          <t>TERMINAL REFINERÍA PAMPILLA</t>
         </is>
       </c>
     </row>
@@ -2026,7 +2026,7 @@
       </c>
       <c r="K29" t="inlineStr">
         <is>
-          <t>Terminal Refinería Pampilla</t>
+          <t>TERMINAL REFINERÍA PAMPILLA</t>
         </is>
       </c>
     </row>
@@ -2081,7 +2081,7 @@
       </c>
       <c r="K30" t="inlineStr">
         <is>
-          <t>Terminal Refinería Pampilla</t>
+          <t>TERMINAL REFINERÍA PAMPILLA</t>
         </is>
       </c>
     </row>
@@ -2136,7 +2136,7 @@
       </c>
       <c r="K31" t="inlineStr">
         <is>
-          <t>Terminal Refinería Pampilla</t>
+          <t>TERMINAL REFINERÍA PAMPILLA</t>
         </is>
       </c>
     </row>
@@ -2191,7 +2191,7 @@
       </c>
       <c r="K32" t="inlineStr">
         <is>
-          <t>Terminal Refinería Pampilla</t>
+          <t>TERMINAL REFINERÍA PAMPILLA</t>
         </is>
       </c>
     </row>
@@ -2246,7 +2246,7 @@
       </c>
       <c r="K33" t="inlineStr">
         <is>
-          <t>Terminal Refinería Pampilla</t>
+          <t>TERMINAL REFINERÍA PAMPILLA</t>
         </is>
       </c>
     </row>
@@ -2301,7 +2301,7 @@
       </c>
       <c r="K34" t="inlineStr">
         <is>
-          <t>Terminal Refinería Pampilla</t>
+          <t>TERMINAL REFINERÍA PAMPILLA</t>
         </is>
       </c>
     </row>
@@ -2356,7 +2356,7 @@
       </c>
       <c r="K35" t="inlineStr">
         <is>
-          <t>Terminal Refinería Pampilla</t>
+          <t>TERMINAL REFINERÍA PAMPILLA</t>
         </is>
       </c>
     </row>
@@ -2411,7 +2411,7 @@
       </c>
       <c r="K36" t="inlineStr">
         <is>
-          <t>Terminal Refinería Pampilla</t>
+          <t>TERMINAL REFINERÍA PAMPILLA</t>
         </is>
       </c>
     </row>
@@ -2466,7 +2466,7 @@
       </c>
       <c r="K37" t="inlineStr">
         <is>
-          <t>Terminal PBF Callao</t>
+          <t>TERMINAL PBF CALLAO</t>
         </is>
       </c>
     </row>
@@ -2521,7 +2521,7 @@
       </c>
       <c r="K38" t="inlineStr">
         <is>
-          <t>Terminal PBF Callao</t>
+          <t>TERMINAL PBF CALLAO</t>
         </is>
       </c>
     </row>
@@ -2576,7 +2576,7 @@
       </c>
       <c r="K39" t="inlineStr">
         <is>
-          <t>Terminal PBF Callao</t>
+          <t>TERMINAL PBF CALLAO</t>
         </is>
       </c>
     </row>
@@ -2631,7 +2631,7 @@
       </c>
       <c r="K40" t="inlineStr">
         <is>
-          <t>Terminal PBF Callao</t>
+          <t>TERMINAL PBF CALLAO</t>
         </is>
       </c>
     </row>
@@ -2686,7 +2686,7 @@
       </c>
       <c r="K41" t="inlineStr">
         <is>
-          <t>Terminal PBF Callao</t>
+          <t>TERMINAL PBF CALLAO</t>
         </is>
       </c>
     </row>
@@ -2741,7 +2741,7 @@
       </c>
       <c r="K42" t="inlineStr">
         <is>
-          <t>Terminal PBF Callao</t>
+          <t>TERMINAL PBF CALLAO</t>
         </is>
       </c>
     </row>
@@ -2796,7 +2796,7 @@
       </c>
       <c r="K43" t="inlineStr">
         <is>
-          <t>Terminal PBF Callao</t>
+          <t>TERMINAL PBF CALLAO</t>
         </is>
       </c>
     </row>
@@ -2851,7 +2851,7 @@
       </c>
       <c r="K44" t="inlineStr">
         <is>
-          <t>Terminal PBF Callao</t>
+          <t>TERMINAL PBF CALLAO</t>
         </is>
       </c>
     </row>
@@ -2906,7 +2906,7 @@
       </c>
       <c r="K45" t="inlineStr">
         <is>
-          <t>Terminal PBF Callao</t>
+          <t>TERMINAL PBF CALLAO</t>
         </is>
       </c>
     </row>
@@ -2961,7 +2961,7 @@
       </c>
       <c r="K46" t="inlineStr">
         <is>
-          <t>Terminal PBF Callao</t>
+          <t>TERMINAL PBF CALLAO</t>
         </is>
       </c>
     </row>
@@ -3016,7 +3016,7 @@
       </c>
       <c r="K47" t="inlineStr">
         <is>
-          <t>Terminal PBF Callao</t>
+          <t>TERMINAL PBF CALLAO</t>
         </is>
       </c>
     </row>
@@ -3071,7 +3071,7 @@
       </c>
       <c r="K48" t="inlineStr">
         <is>
-          <t>Terminal PBF Callao</t>
+          <t>TERMINAL PBF CALLAO</t>
         </is>
       </c>
     </row>
@@ -3126,7 +3126,7 @@
       </c>
       <c r="K49" t="inlineStr">
         <is>
-          <t>Terminal PBF Callao</t>
+          <t>TERMINAL PBF CALLAO</t>
         </is>
       </c>
     </row>
@@ -3181,7 +3181,7 @@
       </c>
       <c r="K50" t="inlineStr">
         <is>
-          <t>Terminal PBF Callao</t>
+          <t>TERMINAL PBF CALLAO</t>
         </is>
       </c>
     </row>
@@ -3236,7 +3236,7 @@
       </c>
       <c r="K51" t="inlineStr">
         <is>
-          <t>Terminal PBF Callao</t>
+          <t>TERMINAL PBF CALLAO</t>
         </is>
       </c>
     </row>
@@ -3291,7 +3291,7 @@
       </c>
       <c r="K52" t="inlineStr">
         <is>
-          <t>Terminal PBF Callao</t>
+          <t>TERMINAL PBF CALLAO</t>
         </is>
       </c>
     </row>
@@ -3346,7 +3346,7 @@
       </c>
       <c r="K53" t="inlineStr">
         <is>
-          <t>Terminal PBF Callao</t>
+          <t>TERMINAL PBF CALLAO</t>
         </is>
       </c>
     </row>
@@ -3401,7 +3401,7 @@
       </c>
       <c r="K54" t="inlineStr">
         <is>
-          <t>Terminal PBF Callao</t>
+          <t>TERMINAL PBF CALLAO</t>
         </is>
       </c>
     </row>
@@ -3456,7 +3456,7 @@
       </c>
       <c r="K55" t="inlineStr">
         <is>
-          <t>Terminal PBF Callao</t>
+          <t>TERMINAL PBF CALLAO</t>
         </is>
       </c>
     </row>
@@ -3511,7 +3511,7 @@
       </c>
       <c r="K56" t="inlineStr">
         <is>
-          <t>Terminal PBF Callao</t>
+          <t>TERMINAL PBF CALLAO</t>
         </is>
       </c>
     </row>
@@ -3566,7 +3566,7 @@
       </c>
       <c r="K57" t="inlineStr">
         <is>
-          <t>Terminal PBF Callao</t>
+          <t>TERMINAL PBF CALLAO</t>
         </is>
       </c>
     </row>
@@ -3621,7 +3621,7 @@
       </c>
       <c r="K58" t="inlineStr">
         <is>
-          <t>Terminal Refinería Pampilla</t>
+          <t>TERMINAL REFINERÍA PAMPILLA</t>
         </is>
       </c>
     </row>
@@ -3676,7 +3676,7 @@
       </c>
       <c r="K59" t="inlineStr">
         <is>
-          <t>Terminal Refinería Pampilla</t>
+          <t>TERMINAL REFINERÍA PAMPILLA</t>
         </is>
       </c>
     </row>
@@ -3731,7 +3731,7 @@
       </c>
       <c r="K60" t="inlineStr">
         <is>
-          <t>Terminal Refinería Pampilla</t>
+          <t>TERMINAL REFINERÍA PAMPILLA</t>
         </is>
       </c>
     </row>
@@ -3786,7 +3786,7 @@
       </c>
       <c r="K61" t="inlineStr">
         <is>
-          <t>Terminal Refinería Pampilla</t>
+          <t>TERMINAL REFINERÍA PAMPILLA</t>
         </is>
       </c>
     </row>
@@ -3841,7 +3841,7 @@
       </c>
       <c r="K62" t="inlineStr">
         <is>
-          <t>Terminal Refinería Conchán</t>
+          <t>TERMINAL REFINERÍA CONCHÁN</t>
         </is>
       </c>
     </row>
@@ -3896,7 +3896,7 @@
       </c>
       <c r="K63" t="inlineStr">
         <is>
-          <t>Terminal Refinería Conchán</t>
+          <t>TERMINAL REFINERÍA CONCHÁN</t>
         </is>
       </c>
     </row>
@@ -3951,7 +3951,7 @@
       </c>
       <c r="K64" t="inlineStr">
         <is>
-          <t>Terminal Refinería Conchán</t>
+          <t>TERMINAL REFINERÍA CONCHÁN</t>
         </is>
       </c>
     </row>
@@ -4006,7 +4006,7 @@
       </c>
       <c r="K65" t="inlineStr">
         <is>
-          <t>Terminal Refinería Conchán</t>
+          <t>TERMINAL REFINERÍA CONCHÁN</t>
         </is>
       </c>
     </row>
@@ -4061,7 +4061,7 @@
       </c>
       <c r="K66" t="inlineStr">
         <is>
-          <t>Terminal Refinería Pampilla</t>
+          <t>TERMINAL REFINERÍA PAMPILLA</t>
         </is>
       </c>
     </row>
@@ -4116,7 +4116,7 @@
       </c>
       <c r="K67" t="inlineStr">
         <is>
-          <t>Terminal Refinería Pampilla</t>
+          <t>TERMINAL REFINERÍA PAMPILLA</t>
         </is>
       </c>
     </row>
@@ -4171,7 +4171,7 @@
       </c>
       <c r="K68" t="inlineStr">
         <is>
-          <t>Terminal Refinería Pampilla</t>
+          <t>TERMINAL REFINERÍA PAMPILLA</t>
         </is>
       </c>
     </row>
@@ -4226,7 +4226,7 @@
       </c>
       <c r="K69" t="inlineStr">
         <is>
-          <t>Terminal Refinería Pampilla</t>
+          <t>TERMINAL REFINERÍA PAMPILLA</t>
         </is>
       </c>
     </row>
@@ -4281,7 +4281,7 @@
       </c>
       <c r="K70" t="inlineStr">
         <is>
-          <t>Terminal Refinería Pampilla</t>
+          <t>TERMINAL REFINERÍA PAMPILLA</t>
         </is>
       </c>
     </row>
@@ -4336,7 +4336,7 @@
       </c>
       <c r="K71" t="inlineStr">
         <is>
-          <t>Terminal Refinería Pampilla</t>
+          <t>TERMINAL REFINERÍA PAMPILLA</t>
         </is>
       </c>
     </row>
@@ -4391,7 +4391,7 @@
       </c>
       <c r="K72" t="inlineStr">
         <is>
-          <t>Terminal Refinería Pampilla</t>
+          <t>TERMINAL REFINERÍA PAMPILLA</t>
         </is>
       </c>
     </row>
@@ -4446,7 +4446,7 @@
       </c>
       <c r="K73" t="inlineStr">
         <is>
-          <t>Terminal Refinería Pampilla</t>
+          <t>TERMINAL REFINERÍA PAMPILLA</t>
         </is>
       </c>
     </row>
@@ -4501,7 +4501,7 @@
       </c>
       <c r="K74" t="inlineStr">
         <is>
-          <t>Terminal Refinería Pampilla</t>
+          <t>TERMINAL REFINERÍA PAMPILLA</t>
         </is>
       </c>
     </row>
@@ -4556,7 +4556,7 @@
       </c>
       <c r="K75" t="inlineStr">
         <is>
-          <t>Terminal Refinería Pampilla</t>
+          <t>TERMINAL REFINERÍA PAMPILLA</t>
         </is>
       </c>
     </row>
@@ -4611,7 +4611,7 @@
       </c>
       <c r="K76" t="inlineStr">
         <is>
-          <t>Terminal Refinería Pampilla</t>
+          <t>TERMINAL REFINERÍA PAMPILLA</t>
         </is>
       </c>
     </row>
@@ -4666,7 +4666,7 @@
       </c>
       <c r="K77" t="inlineStr">
         <is>
-          <t>Terminal Refinería Pampilla</t>
+          <t>TERMINAL REFINERÍA PAMPILLA</t>
         </is>
       </c>
     </row>
@@ -4721,7 +4721,7 @@
       </c>
       <c r="K78" t="inlineStr">
         <is>
-          <t>Terminal Refinería Pampilla</t>
+          <t>TERMINAL REFINERÍA PAMPILLA</t>
         </is>
       </c>
     </row>
@@ -4776,7 +4776,7 @@
       </c>
       <c r="K79" t="inlineStr">
         <is>
-          <t>Terminal Refinería Pampilla</t>
+          <t>TERMINAL REFINERÍA PAMPILLA</t>
         </is>
       </c>
     </row>
@@ -4831,7 +4831,7 @@
       </c>
       <c r="K80" t="inlineStr">
         <is>
-          <t>Terminal Refinería Pampilla</t>
+          <t>TERMINAL REFINERÍA PAMPILLA</t>
         </is>
       </c>
     </row>
@@ -4886,7 +4886,7 @@
       </c>
       <c r="K81" t="inlineStr">
         <is>
-          <t>Terminal Refinería Pampilla</t>
+          <t>TERMINAL REFINERÍA PAMPILLA</t>
         </is>
       </c>
     </row>
@@ -4941,7 +4941,7 @@
       </c>
       <c r="K82" t="inlineStr">
         <is>
-          <t>Terminal Refinería Pampilla</t>
+          <t>TERMINAL REFINERÍA PAMPILLA</t>
         </is>
       </c>
     </row>
@@ -4996,7 +4996,7 @@
       </c>
       <c r="K83" t="inlineStr">
         <is>
-          <t>Terminal Refinería Pampilla</t>
+          <t>TERMINAL REFINERÍA PAMPILLA</t>
         </is>
       </c>
     </row>
@@ -5051,7 +5051,7 @@
       </c>
       <c r="K84" t="inlineStr">
         <is>
-          <t>Terminal Refinería Pampilla</t>
+          <t>TERMINAL REFINERÍA PAMPILLA</t>
         </is>
       </c>
     </row>
@@ -5106,7 +5106,7 @@
       </c>
       <c r="K85" t="inlineStr">
         <is>
-          <t>Terminal PBF Callao</t>
+          <t>TERMINAL PBF CALLAO</t>
         </is>
       </c>
     </row>
@@ -5161,7 +5161,7 @@
       </c>
       <c r="K86" t="inlineStr">
         <is>
-          <t>Terminal PBF Callao</t>
+          <t>TERMINAL PBF CALLAO</t>
         </is>
       </c>
     </row>
@@ -5216,7 +5216,7 @@
       </c>
       <c r="K87" t="inlineStr">
         <is>
-          <t>Terminal PBF Callao</t>
+          <t>TERMINAL PBF CALLAO</t>
         </is>
       </c>
     </row>
@@ -5271,7 +5271,7 @@
       </c>
       <c r="K88" t="inlineStr">
         <is>
-          <t>Terminal PBF Callao</t>
+          <t>TERMINAL PBF CALLAO</t>
         </is>
       </c>
     </row>
@@ -5326,7 +5326,7 @@
       </c>
       <c r="K89" t="inlineStr">
         <is>
-          <t>Terminal PBF Callao</t>
+          <t>TERMINAL PBF CALLAO</t>
         </is>
       </c>
     </row>
@@ -5381,7 +5381,7 @@
       </c>
       <c r="K90" t="inlineStr">
         <is>
-          <t>Terminal PBF Callao</t>
+          <t>TERMINAL PBF CALLAO</t>
         </is>
       </c>
     </row>
@@ -5436,7 +5436,7 @@
       </c>
       <c r="K91" t="inlineStr">
         <is>
-          <t>Terminal PBF Callao</t>
+          <t>TERMINAL PBF CALLAO</t>
         </is>
       </c>
     </row>
@@ -5491,7 +5491,7 @@
       </c>
       <c r="K92" t="inlineStr">
         <is>
-          <t>Terminal PBF Callao</t>
+          <t>TERMINAL PBF CALLAO</t>
         </is>
       </c>
     </row>
@@ -5546,7 +5546,7 @@
       </c>
       <c r="K93" t="inlineStr">
         <is>
-          <t>Terminal PBF Callao</t>
+          <t>TERMINAL PBF CALLAO</t>
         </is>
       </c>
     </row>
@@ -5601,7 +5601,7 @@
       </c>
       <c r="K94" t="inlineStr">
         <is>
-          <t>Terminal PBF Callao</t>
+          <t>TERMINAL PBF CALLAO</t>
         </is>
       </c>
     </row>
@@ -5656,7 +5656,7 @@
       </c>
       <c r="K95" t="inlineStr">
         <is>
-          <t>Terminal PBF Callao</t>
+          <t>TERMINAL PBF CALLAO</t>
         </is>
       </c>
     </row>
@@ -5711,7 +5711,7 @@
       </c>
       <c r="K96" t="inlineStr">
         <is>
-          <t>Terminal PBF Callao</t>
+          <t>TERMINAL PBF CALLAO</t>
         </is>
       </c>
     </row>
@@ -5766,7 +5766,7 @@
       </c>
       <c r="K97" t="inlineStr">
         <is>
-          <t>Terminal PBF Callao</t>
+          <t>TERMINAL PBF CALLAO</t>
         </is>
       </c>
     </row>
@@ -5821,7 +5821,7 @@
       </c>
       <c r="K98" t="inlineStr">
         <is>
-          <t>Terminal PBF Callao</t>
+          <t>TERMINAL PBF CALLAO</t>
         </is>
       </c>
     </row>
@@ -5876,7 +5876,7 @@
       </c>
       <c r="K99" t="inlineStr">
         <is>
-          <t>Terminal PBF Callao</t>
+          <t>TERMINAL PBF CALLAO</t>
         </is>
       </c>
     </row>
@@ -5931,7 +5931,7 @@
       </c>
       <c r="K100" t="inlineStr">
         <is>
-          <t>Terminal PBF Callao</t>
+          <t>TERMINAL PBF CALLAO</t>
         </is>
       </c>
     </row>
@@ -5986,7 +5986,7 @@
       </c>
       <c r="K101" t="inlineStr">
         <is>
-          <t>Terminal PBF Callao</t>
+          <t>TERMINAL PBF CALLAO</t>
         </is>
       </c>
     </row>
@@ -6041,7 +6041,7 @@
       </c>
       <c r="K102" t="inlineStr">
         <is>
-          <t>Terminal PBF Callao</t>
+          <t>TERMINAL PBF CALLAO</t>
         </is>
       </c>
     </row>
@@ -6096,7 +6096,7 @@
       </c>
       <c r="K103" t="inlineStr">
         <is>
-          <t>Terminal PBF Callao</t>
+          <t>TERMINAL PBF CALLAO</t>
         </is>
       </c>
     </row>
@@ -6151,7 +6151,7 @@
       </c>
       <c r="K104" t="inlineStr">
         <is>
-          <t>Terminal PBF Callao</t>
+          <t>TERMINAL PBF CALLAO</t>
         </is>
       </c>
     </row>
@@ -6206,7 +6206,7 @@
       </c>
       <c r="K105" t="inlineStr">
         <is>
-          <t>Terminal PBF Callao</t>
+          <t>TERMINAL PBF CALLAO</t>
         </is>
       </c>
     </row>
@@ -6261,7 +6261,7 @@
       </c>
       <c r="K106" t="inlineStr">
         <is>
-          <t>Terminal PBF Callao</t>
+          <t>TERMINAL PBF CALLAO</t>
         </is>
       </c>
     </row>
@@ -6316,7 +6316,7 @@
       </c>
       <c r="K107" t="inlineStr">
         <is>
-          <t>Terminal PBF Callao</t>
+          <t>TERMINAL PBF CALLAO</t>
         </is>
       </c>
     </row>
@@ -6371,7 +6371,7 @@
       </c>
       <c r="K108" t="inlineStr">
         <is>
-          <t>Terminal PBF Callao</t>
+          <t>TERMINAL PBF CALLAO</t>
         </is>
       </c>
     </row>
@@ -6426,7 +6426,7 @@
       </c>
       <c r="K109" t="inlineStr">
         <is>
-          <t>Terminal PBF Callao</t>
+          <t>TERMINAL PBF CALLAO</t>
         </is>
       </c>
     </row>
@@ -6481,7 +6481,7 @@
       </c>
       <c r="K110" t="inlineStr">
         <is>
-          <t>Terminal Refinería Pampilla</t>
+          <t>TERMINAL REFINERÍA PAMPILLA</t>
         </is>
       </c>
     </row>
@@ -6536,7 +6536,7 @@
       </c>
       <c r="K111" t="inlineStr">
         <is>
-          <t>Terminal Refinería Pampilla</t>
+          <t>TERMINAL REFINERÍA PAMPILLA</t>
         </is>
       </c>
     </row>
@@ -6591,7 +6591,7 @@
       </c>
       <c r="K112" t="inlineStr">
         <is>
-          <t>Terminal Refinería Pampilla</t>
+          <t>TERMINAL REFINERÍA PAMPILLA</t>
         </is>
       </c>
     </row>
@@ -6646,7 +6646,7 @@
       </c>
       <c r="K113" t="inlineStr">
         <is>
-          <t>Terminal Refinería Pampilla</t>
+          <t>TERMINAL REFINERÍA PAMPILLA</t>
         </is>
       </c>
     </row>
@@ -6701,7 +6701,7 @@
       </c>
       <c r="K114" t="inlineStr">
         <is>
-          <t>Terminal Refinería Pampilla</t>
+          <t>TERMINAL REFINERÍA PAMPILLA</t>
         </is>
       </c>
     </row>
@@ -6756,7 +6756,7 @@
       </c>
       <c r="K115" t="inlineStr">
         <is>
-          <t>Terminal Refinería Pampilla</t>
+          <t>TERMINAL REFINERÍA PAMPILLA</t>
         </is>
       </c>
     </row>
@@ -6811,7 +6811,7 @@
       </c>
       <c r="K116" t="inlineStr">
         <is>
-          <t>Terminal PBF Callao</t>
+          <t>TERMINAL PBF CALLAO</t>
         </is>
       </c>
     </row>
@@ -6866,7 +6866,7 @@
       </c>
       <c r="K117" t="inlineStr">
         <is>
-          <t>Terminal PBF Callao</t>
+          <t>TERMINAL PBF CALLAO</t>
         </is>
       </c>
     </row>
@@ -6921,7 +6921,7 @@
       </c>
       <c r="K118" t="inlineStr">
         <is>
-          <t>Terminal PBF Callao</t>
+          <t>TERMINAL PBF CALLAO</t>
         </is>
       </c>
     </row>
@@ -6976,7 +6976,7 @@
       </c>
       <c r="K119" t="inlineStr">
         <is>
-          <t>Terminal PBF Callao</t>
+          <t>TERMINAL PBF CALLAO</t>
         </is>
       </c>
     </row>
@@ -7031,7 +7031,7 @@
       </c>
       <c r="K120" t="inlineStr">
         <is>
-          <t>Terminal Refinería Pampilla</t>
+          <t>TERMINAL REFINERÍA PAMPILLA</t>
         </is>
       </c>
     </row>
@@ -7086,7 +7086,7 @@
       </c>
       <c r="K121" t="inlineStr">
         <is>
-          <t>Terminal Refinería Pampilla</t>
+          <t>TERMINAL REFINERÍA PAMPILLA</t>
         </is>
       </c>
     </row>
@@ -7141,7 +7141,7 @@
       </c>
       <c r="K122" t="inlineStr">
         <is>
-          <t>Terminal Refinería Pampilla</t>
+          <t>TERMINAL REFINERÍA PAMPILLA</t>
         </is>
       </c>
     </row>
@@ -7196,7 +7196,7 @@
       </c>
       <c r="K123" t="inlineStr">
         <is>
-          <t>Terminal Refinería Pampilla</t>
+          <t>TERMINAL REFINERÍA PAMPILLA</t>
         </is>
       </c>
     </row>
@@ -7251,7 +7251,7 @@
       </c>
       <c r="K124" t="inlineStr">
         <is>
-          <t>Terminal Refinería Pampilla</t>
+          <t>TERMINAL REFINERÍA PAMPILLA</t>
         </is>
       </c>
     </row>
@@ -7306,7 +7306,7 @@
       </c>
       <c r="K125" t="inlineStr">
         <is>
-          <t>Terminal Refinería Pampilla</t>
+          <t>TERMINAL REFINERÍA PAMPILLA</t>
         </is>
       </c>
     </row>
@@ -7361,7 +7361,7 @@
       </c>
       <c r="K126" t="inlineStr">
         <is>
-          <t>Terminal Refinería Conchán</t>
+          <t>TERMINAL REFINERÍA CONCHÁN</t>
         </is>
       </c>
     </row>
@@ -7416,7 +7416,7 @@
       </c>
       <c r="K127" t="inlineStr">
         <is>
-          <t>Terminal Refinería Conchán</t>
+          <t>TERMINAL REFINERÍA CONCHÁN</t>
         </is>
       </c>
     </row>
@@ -7471,7 +7471,7 @@
       </c>
       <c r="K128" t="inlineStr">
         <is>
-          <t>Terminal Refinería Conchán</t>
+          <t>TERMINAL REFINERÍA CONCHÁN</t>
         </is>
       </c>
     </row>
@@ -7526,7 +7526,7 @@
       </c>
       <c r="K129" t="inlineStr">
         <is>
-          <t>Terminal Refinería Conchán</t>
+          <t>TERMINAL REFINERÍA CONCHÁN</t>
         </is>
       </c>
     </row>
@@ -7581,7 +7581,7 @@
       </c>
       <c r="K130" t="inlineStr">
         <is>
-          <t>Terminal Refinería Conchán</t>
+          <t>TERMINAL REFINERÍA CONCHÁN</t>
         </is>
       </c>
     </row>
@@ -7636,7 +7636,7 @@
       </c>
       <c r="K131" t="inlineStr">
         <is>
-          <t>Terminal Refinería Conchán</t>
+          <t>TERMINAL REFINERÍA CONCHÁN</t>
         </is>
       </c>
     </row>
@@ -7691,7 +7691,7 @@
       </c>
       <c r="K132" t="inlineStr">
         <is>
-          <t>Terminal Refinería Conchán</t>
+          <t>TERMINAL REFINERÍA CONCHÁN</t>
         </is>
       </c>
     </row>
@@ -7746,7 +7746,7 @@
       </c>
       <c r="K133" t="inlineStr">
         <is>
-          <t>Terminal Refinería Conchán</t>
+          <t>TERMINAL REFINERÍA CONCHÁN</t>
         </is>
       </c>
     </row>
@@ -7801,7 +7801,7 @@
       </c>
       <c r="K134" t="inlineStr">
         <is>
-          <t>Terminal Refinería Conchán</t>
+          <t>TERMINAL REFINERÍA CONCHÁN</t>
         </is>
       </c>
     </row>
@@ -7856,7 +7856,7 @@
       </c>
       <c r="K135" t="inlineStr">
         <is>
-          <t>Terminal Refinería Conchán</t>
+          <t>TERMINAL REFINERÍA CONCHÁN</t>
         </is>
       </c>
     </row>
@@ -7911,7 +7911,7 @@
       </c>
       <c r="K136" t="inlineStr">
         <is>
-          <t>Terminal Refinería Conchán</t>
+          <t>TERMINAL REFINERÍA CONCHÁN</t>
         </is>
       </c>
     </row>
@@ -7966,7 +7966,7 @@
       </c>
       <c r="K137" t="inlineStr">
         <is>
-          <t>Terminal Refinería Pampilla</t>
+          <t>TERMINAL REFINERÍA PAMPILLA</t>
         </is>
       </c>
     </row>
@@ -8021,7 +8021,7 @@
       </c>
       <c r="K138" t="inlineStr">
         <is>
-          <t>Terminal Refinería Pampilla</t>
+          <t>TERMINAL REFINERÍA PAMPILLA</t>
         </is>
       </c>
     </row>
@@ -8076,7 +8076,7 @@
       </c>
       <c r="K139" t="inlineStr">
         <is>
-          <t>Terminal Refinería Pampilla</t>
+          <t>TERMINAL REFINERÍA PAMPILLA</t>
         </is>
       </c>
     </row>
@@ -8131,7 +8131,7 @@
       </c>
       <c r="K140" t="inlineStr">
         <is>
-          <t>Terminal Refinería Pampilla</t>
+          <t>TERMINAL REFINERÍA PAMPILLA</t>
         </is>
       </c>
     </row>
@@ -8186,7 +8186,7 @@
       </c>
       <c r="K141" t="inlineStr">
         <is>
-          <t>Terminal Refinería Pampilla</t>
+          <t>TERMINAL REFINERÍA PAMPILLA</t>
         </is>
       </c>
     </row>
@@ -8241,7 +8241,7 @@
       </c>
       <c r="K142" t="inlineStr">
         <is>
-          <t>Terminal Refinería Pampilla</t>
+          <t>TERMINAL REFINERÍA PAMPILLA</t>
         </is>
       </c>
     </row>
@@ -8296,7 +8296,7 @@
       </c>
       <c r="K143" t="inlineStr">
         <is>
-          <t>Terminal PBF Callao</t>
+          <t>TERMINAL PBF CALLAO</t>
         </is>
       </c>
     </row>
@@ -8351,7 +8351,7 @@
       </c>
       <c r="K144" t="inlineStr">
         <is>
-          <t>Terminal PBF Callao</t>
+          <t>TERMINAL PBF CALLAO</t>
         </is>
       </c>
     </row>
@@ -8406,7 +8406,7 @@
       </c>
       <c r="K145" t="inlineStr">
         <is>
-          <t>Terminal PBF Callao</t>
+          <t>TERMINAL PBF CALLAO</t>
         </is>
       </c>
     </row>
@@ -8461,7 +8461,7 @@
       </c>
       <c r="K146" t="inlineStr">
         <is>
-          <t>Terminal PBF Callao</t>
+          <t>TERMINAL PBF CALLAO</t>
         </is>
       </c>
     </row>
@@ -8516,7 +8516,7 @@
       </c>
       <c r="K147" t="inlineStr">
         <is>
-          <t>Terminal PBF Callao</t>
+          <t>TERMINAL PBF CALLAO</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Se agrega restricción de cada compartimento solo va a un cliente
</commit_message>
<xml_diff>
--- a/datos_intermedios/Data_Filtrada_COESTI.xlsx
+++ b/datos_intermedios/Data_Filtrada_COESTI.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L114"/>
+  <dimension ref="A1:L111"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1518,27 +1518,27 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>4501033983</t>
+          <t>4501031892</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>P181</t>
+          <t>P327</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>E/S PUNTA HERMOSA</t>
+          <t>E/S ZARATE</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Carr. Panamericana Sur, 1S, Lima</t>
+          <t>Av. Malecón Checa, San Juan de Lurigancho 15401</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>PUNTA HERMOSA</t>
+          <t>ZARATE</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
@@ -1552,16 +1552,16 @@
         </is>
       </c>
       <c r="H19" t="n">
-        <v>1750</v>
+        <v>1500</v>
       </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>40002019</t>
+          <t>40002039</t>
         </is>
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>MAX-D DIESEL B5 S50 UV</t>
+          <t>PRIMAX GASOHOL 90</t>
         </is>
       </c>
       <c r="K19" t="inlineStr">
@@ -1578,27 +1578,27 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>4501033988</t>
+          <t>4501031892</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>P181</t>
+          <t>P327</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>E/S PUNTA HERMOSA</t>
+          <t>E/S ZARATE</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>Carr. Panamericana Sur, 1S, Lima</t>
+          <t>Av. Malecón Checa, San Juan de Lurigancho 15401</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>PUNTA HERMOSA</t>
+          <t>ZARATE</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
@@ -1612,16 +1612,16 @@
         </is>
       </c>
       <c r="H20" t="n">
-        <v>1750</v>
+        <v>1500</v>
       </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t>40002019</t>
+          <t>40002047</t>
         </is>
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>MAX-D DIESEL B5 S50 UV</t>
+          <t>PRIMAX GASOHOL 95</t>
         </is>
       </c>
       <c r="K20" t="inlineStr">
@@ -1638,27 +1638,27 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>4501033990</t>
+          <t>4501034405</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>P181</t>
+          <t>P255</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>E/S PUNTA HERMOSA</t>
+          <t>E/S LURIGANCHO</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Carr. Panamericana Sur, 1S, Lima</t>
+          <t>Av. Lurigancho 1175, San Juan de Lurigancho 15427</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>PUNTA HERMOSA</t>
+          <t>CANTO GRANDE</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
@@ -1672,7 +1672,7 @@
         </is>
       </c>
       <c r="H21" t="n">
-        <v>500</v>
+        <v>1000</v>
       </c>
       <c r="I21" t="inlineStr">
         <is>
@@ -1698,27 +1698,27 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>4501031892</t>
+          <t>4501034468</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>P327</t>
+          <t>P223</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>E/S ZARATE</t>
+          <t>E/S FELVERANA</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Av. Malecón Checa, San Juan de Lurigancho 15401</t>
+          <t>Av. Nicolás Ayllón 2162, Ate 15022</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>ZARATE</t>
+          <t>ATE</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
@@ -1732,16 +1732,16 @@
         </is>
       </c>
       <c r="H22" t="n">
-        <v>1500</v>
+        <v>9000</v>
       </c>
       <c r="I22" t="inlineStr">
         <is>
-          <t>40002039</t>
+          <t>40002019</t>
         </is>
       </c>
       <c r="J22" t="inlineStr">
         <is>
-          <t>PRIMAX GASOHOL 90</t>
+          <t>MAX-D DIESEL B5 S50 UV</t>
         </is>
       </c>
       <c r="K22" t="inlineStr">
@@ -1758,27 +1758,27 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>4501031892</t>
+          <t>4501034544</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>P327</t>
+          <t>P275</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>E/S ZARATE</t>
+          <t>E/S PANSUR</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>Av. Malecón Checa, San Juan de Lurigancho 15401</t>
+          <t>Km, Antigua Panamericana Sur 30, Lurín</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>ZARATE</t>
+          <t>LURIN</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
@@ -1792,53 +1792,53 @@
         </is>
       </c>
       <c r="H23" t="n">
-        <v>1500</v>
+        <v>2000</v>
       </c>
       <c r="I23" t="inlineStr">
         <is>
-          <t>40002047</t>
+          <t>40002019</t>
         </is>
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>PRIMAX GASOHOL 95</t>
+          <t>MAX-D DIESEL B5 S50 UV</t>
         </is>
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>P611</t>
+          <t>P614</t>
         </is>
       </c>
       <c r="L23" t="inlineStr">
         <is>
-          <t>TERMINAL REFINERÍA PAMPILLA</t>
+          <t>TERMINAL PBF CALLAO</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>4501034405</t>
+          <t>4501034545</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>P255</t>
+          <t>P275</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>E/S LURIGANCHO</t>
+          <t>E/S PANSUR</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>Av. Lurigancho 1175, San Juan de Lurigancho 15427</t>
+          <t>Km, Antigua Panamericana Sur 30, Lurín</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>CANTO GRANDE</t>
+          <t>LURIN</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
@@ -1852,7 +1852,7 @@
         </is>
       </c>
       <c r="H24" t="n">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="I24" t="inlineStr">
         <is>
@@ -1866,39 +1866,39 @@
       </c>
       <c r="K24" t="inlineStr">
         <is>
-          <t>P611</t>
+          <t>P614</t>
         </is>
       </c>
       <c r="L24" t="inlineStr">
         <is>
-          <t>TERMINAL REFINERÍA PAMPILLA</t>
+          <t>TERMINAL PBF CALLAO</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>4501034468</t>
+          <t>4501034545</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>P223</t>
+          <t>P275</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>E/S FELVERANA</t>
+          <t>E/S PANSUR</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>Av. Nicolás Ayllón 2162, Ate 15022</t>
+          <t>Km, Antigua Panamericana Sur 30, Lurín</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>ATE</t>
+          <t>LURIN</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
@@ -1912,33 +1912,33 @@
         </is>
       </c>
       <c r="H25" t="n">
-        <v>9000</v>
+        <v>1000</v>
       </c>
       <c r="I25" t="inlineStr">
         <is>
-          <t>40002019</t>
+          <t>40002047</t>
         </is>
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>MAX-D DIESEL B5 S50 UV</t>
+          <t>PRIMAX GASOHOL 95</t>
         </is>
       </c>
       <c r="K25" t="inlineStr">
         <is>
-          <t>P611</t>
+          <t>P614</t>
         </is>
       </c>
       <c r="L25" t="inlineStr">
         <is>
-          <t>TERMINAL REFINERÍA PAMPILLA</t>
+          <t>TERMINAL PBF CALLAO</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>4501034544</t>
+          <t>4501034545</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -1972,16 +1972,16 @@
         </is>
       </c>
       <c r="H26" t="n">
-        <v>2000</v>
+        <v>1000</v>
       </c>
       <c r="I26" t="inlineStr">
         <is>
-          <t>40002019</t>
+          <t>40002055</t>
         </is>
       </c>
       <c r="J26" t="inlineStr">
         <is>
-          <t>MAX-D DIESEL B5 S50 UV</t>
+          <t>G-PRIX GASOHOL 97</t>
         </is>
       </c>
       <c r="K26" t="inlineStr">
@@ -1998,32 +1998,32 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>4501034545</t>
+          <t>4501034542</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>P275</t>
+          <t>P193</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>E/S PANSUR</t>
+          <t>E/S CHILCA</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>Km, Antigua Panamericana Sur 30, Lurín</t>
+          <t>1S, Chilca 15871</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>LURIN</t>
+          <t>CHILCA</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>LIMA</t>
+          <t>CAÑETE</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
@@ -2032,7 +2032,7 @@
         </is>
       </c>
       <c r="H27" t="n">
-        <v>500</v>
+        <v>1500</v>
       </c>
       <c r="I27" t="inlineStr">
         <is>
@@ -2058,32 +2058,32 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>4501034545</t>
+          <t>4501034542</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>P275</t>
+          <t>P193</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>E/S PANSUR</t>
+          <t>E/S CHILCA</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>Km, Antigua Panamericana Sur 30, Lurín</t>
+          <t>1S, Chilca 15871</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>LURIN</t>
+          <t>CHILCA</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>LIMA</t>
+          <t>CAÑETE</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
@@ -2092,7 +2092,7 @@
         </is>
       </c>
       <c r="H28" t="n">
-        <v>1000</v>
+        <v>1500</v>
       </c>
       <c r="I28" t="inlineStr">
         <is>
@@ -2118,32 +2118,32 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>4501034545</t>
+          <t>4501034542</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>P275</t>
+          <t>P193</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>E/S PANSUR</t>
+          <t>E/S CHILCA</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>Km, Antigua Panamericana Sur 30, Lurín</t>
+          <t>1S, Chilca 15871</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>LURIN</t>
+          <t>CHILCA</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>LIMA</t>
+          <t>CAÑETE</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
@@ -2178,32 +2178,32 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>4501034542</t>
+          <t>4501034587</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>P193</t>
+          <t>P124</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>E/S CHILCA</t>
+          <t>E/S AREQUIPA 1</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>1S, Chilca 15871</t>
+          <t>Av. Arequipa 3325, San Isidro 15046</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>CHILCA</t>
+          <t>LINCE</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>CAÑETE</t>
+          <t>LIMA</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
@@ -2212,7 +2212,7 @@
         </is>
       </c>
       <c r="H30" t="n">
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="I30" t="inlineStr">
         <is>
@@ -2238,32 +2238,32 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>4501034542</t>
+          <t>4501034587</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>P193</t>
+          <t>P124</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>E/S CHILCA</t>
+          <t>E/S AREQUIPA 1</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>1S, Chilca 15871</t>
+          <t>Av. Arequipa 3325, San Isidro 15046</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>CHILCA</t>
+          <t>LINCE</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>CAÑETE</t>
+          <t>LIMA</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
@@ -2272,7 +2272,7 @@
         </is>
       </c>
       <c r="H31" t="n">
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="I31" t="inlineStr">
         <is>
@@ -2298,32 +2298,32 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>4501034542</t>
+          <t>4501034587</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>P193</t>
+          <t>P124</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>E/S CHILCA</t>
+          <t>E/S AREQUIPA 1</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>1S, Chilca 15871</t>
+          <t>Av. Arequipa 3325, San Isidro 15046</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>CHILCA</t>
+          <t>LINCE</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>CAÑETE</t>
+          <t>LIMA</t>
         </is>
       </c>
       <c r="G32" t="inlineStr">
@@ -2358,27 +2358,27 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>4501034587</t>
+          <t>4501034586</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>P124</t>
+          <t>P133</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>E/S AREQUIPA 1</t>
+          <t>E/S ARMENDARIZ</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>Av. Arequipa 3325, San Isidro 15046</t>
+          <t>Armendariz 575, Miraflores 15074</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>LINCE</t>
+          <t>MIRAFLORES</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
@@ -2418,27 +2418,27 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>4501034587</t>
+          <t>4501034586</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>P124</t>
+          <t>P133</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>E/S AREQUIPA 1</t>
+          <t>E/S ARMENDARIZ</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>Av. Arequipa 3325, San Isidro 15046</t>
+          <t>Armendariz 575, Miraflores 15074</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>LINCE</t>
+          <t>MIRAFLORES</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
@@ -2452,7 +2452,7 @@
         </is>
       </c>
       <c r="H34" t="n">
-        <v>1000</v>
+        <v>2000</v>
       </c>
       <c r="I34" t="inlineStr">
         <is>
@@ -2478,27 +2478,27 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>4501034587</t>
+          <t>4501034586</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>P124</t>
+          <t>P133</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>E/S AREQUIPA 1</t>
+          <t>E/S ARMENDARIZ</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>Av. Arequipa 3325, San Isidro 15046</t>
+          <t>Armendariz 575, Miraflores 15074</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>LINCE</t>
+          <t>MIRAFLORES</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
@@ -2538,22 +2538,22 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>4501034586</t>
+          <t>4501034583</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>P133</t>
+          <t>P285</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>E/S ARMENDARIZ</t>
+          <t>E/S REPÚBLICA</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>Armendariz 575, Miraflores 15074</t>
+          <t>Av. Andrés Aramburú 390, Miraflores 15046</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
@@ -2572,16 +2572,16 @@
         </is>
       </c>
       <c r="H36" t="n">
-        <v>1000</v>
+        <v>1500</v>
       </c>
       <c r="I36" t="inlineStr">
         <is>
-          <t>40002039</t>
+          <t>40002019</t>
         </is>
       </c>
       <c r="J36" t="inlineStr">
         <is>
-          <t>PRIMAX GASOHOL 90</t>
+          <t>MAX-D DIESEL B5 S50 UV</t>
         </is>
       </c>
       <c r="K36" t="inlineStr">
@@ -2598,22 +2598,22 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>4501034586</t>
+          <t>4501034585</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>P133</t>
+          <t>P285</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>E/S ARMENDARIZ</t>
+          <t>E/S REPÚBLICA</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>Armendariz 575, Miraflores 15074</t>
+          <t>Av. Andrés Aramburú 390, Miraflores 15046</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
@@ -2636,12 +2636,12 @@
       </c>
       <c r="I37" t="inlineStr">
         <is>
-          <t>40002047</t>
+          <t>40002039</t>
         </is>
       </c>
       <c r="J37" t="inlineStr">
         <is>
-          <t>PRIMAX GASOHOL 95</t>
+          <t>PRIMAX GASOHOL 90</t>
         </is>
       </c>
       <c r="K37" t="inlineStr">
@@ -2658,22 +2658,22 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>4501034586</t>
+          <t>4501034585</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>P133</t>
+          <t>P285</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>E/S ARMENDARIZ</t>
+          <t>E/S REPÚBLICA</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>Armendariz 575, Miraflores 15074</t>
+          <t>Av. Andrés Aramburú 390, Miraflores 15046</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
@@ -2692,16 +2692,16 @@
         </is>
       </c>
       <c r="H38" t="n">
-        <v>1000</v>
+        <v>2000</v>
       </c>
       <c r="I38" t="inlineStr">
         <is>
-          <t>40002055</t>
+          <t>40002047</t>
         </is>
       </c>
       <c r="J38" t="inlineStr">
         <is>
-          <t>G-PRIX GASOHOL 97</t>
+          <t>PRIMAX GASOHOL 95</t>
         </is>
       </c>
       <c r="K38" t="inlineStr">
@@ -2718,27 +2718,27 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>4501034583</t>
+          <t>4501031894</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>P285</t>
+          <t>P101</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>E/S REPÚBLICA</t>
+          <t>E/S MIGUEL ANGEL</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>Av. Andrés Aramburú 390, Miraflores 15046</t>
+          <t>Av. Lima 2000, Villa María del Triunfo 15816</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>MIRAFLORES</t>
+          <t>VILLA EL SALVADOR</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
@@ -2766,39 +2766,39 @@
       </c>
       <c r="K39" t="inlineStr">
         <is>
-          <t>P614</t>
+          <t>P611</t>
         </is>
       </c>
       <c r="L39" t="inlineStr">
         <is>
-          <t>TERMINAL PBF CALLAO</t>
+          <t>TERMINAL REFINERÍA PAMPILLA</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>4501034585</t>
+          <t>4501031895</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>P285</t>
+          <t>P101</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>E/S REPÚBLICA</t>
+          <t>E/S MIGUEL ANGEL</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>Av. Andrés Aramburú 390, Miraflores 15046</t>
+          <t>Av. Lima 2000, Villa María del Triunfo 15816</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>MIRAFLORES</t>
+          <t>VILLA EL SALVADOR</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
@@ -2826,39 +2826,39 @@
       </c>
       <c r="K40" t="inlineStr">
         <is>
-          <t>P614</t>
+          <t>P611</t>
         </is>
       </c>
       <c r="L40" t="inlineStr">
         <is>
-          <t>TERMINAL PBF CALLAO</t>
+          <t>TERMINAL REFINERÍA PAMPILLA</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>4501034585</t>
+          <t>4501031895</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>P285</t>
+          <t>P101</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>E/S REPÚBLICA</t>
+          <t>E/S MIGUEL ANGEL</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>Av. Andrés Aramburú 390, Miraflores 15046</t>
+          <t>Av. Lima 2000, Villa María del Triunfo 15816</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>MIRAFLORES</t>
+          <t>VILLA EL SALVADOR</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
@@ -2872,7 +2872,7 @@
         </is>
       </c>
       <c r="H41" t="n">
-        <v>2000</v>
+        <v>500</v>
       </c>
       <c r="I41" t="inlineStr">
         <is>
@@ -2886,39 +2886,39 @@
       </c>
       <c r="K41" t="inlineStr">
         <is>
-          <t>P614</t>
+          <t>P611</t>
         </is>
       </c>
       <c r="L41" t="inlineStr">
         <is>
-          <t>TERMINAL PBF CALLAO</t>
+          <t>TERMINAL REFINERÍA PAMPILLA</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>4501031894</t>
+          <t>4501031944</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>P101</t>
+          <t>P125</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>E/S MIGUEL ANGEL</t>
+          <t>E/S LOLESA</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>Av. Lima 2000, Villa María del Triunfo 15816</t>
+          <t>Av. Francisco Pizarro Cdra. 9, Rímac 15094</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>VILLA EL SALVADOR</t>
+          <t>RÍMAC</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
@@ -2932,16 +2932,16 @@
         </is>
       </c>
       <c r="H42" t="n">
-        <v>1500</v>
+        <v>2000</v>
       </c>
       <c r="I42" t="inlineStr">
         <is>
-          <t>40002019</t>
+          <t>40002023</t>
         </is>
       </c>
       <c r="J42" t="inlineStr">
         <is>
-          <t>MAX-D DIESEL B5 S50 UV</t>
+          <t>ENDURA DIESEL B5 S50 UV</t>
         </is>
       </c>
       <c r="K42" t="inlineStr">
@@ -2958,27 +2958,27 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>4501031895</t>
+          <t>4501031945</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>P101</t>
+          <t>P125</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>E/S MIGUEL ANGEL</t>
+          <t>E/S LOLESA</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>Av. Lima 2000, Villa María del Triunfo 15816</t>
+          <t>Av. Francisco Pizarro Cdra. 9, Rímac 15094</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>VILLA EL SALVADOR</t>
+          <t>RÍMAC</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
@@ -2992,16 +2992,16 @@
         </is>
       </c>
       <c r="H43" t="n">
-        <v>2000</v>
+        <v>1000</v>
       </c>
       <c r="I43" t="inlineStr">
         <is>
-          <t>40002039</t>
+          <t>40002041</t>
         </is>
       </c>
       <c r="J43" t="inlineStr">
         <is>
-          <t>PRIMAX GASOHOL 90</t>
+          <t>EXELON GASOHOL 90</t>
         </is>
       </c>
       <c r="K43" t="inlineStr">
@@ -3018,27 +3018,27 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>4501031895</t>
+          <t>4501031945</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>P101</t>
+          <t>P125</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>E/S MIGUEL ANGEL</t>
+          <t>E/S LOLESA</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>Av. Lima 2000, Villa María del Triunfo 15816</t>
+          <t>Av. Francisco Pizarro Cdra. 9, Rímac 15094</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>VILLA EL SALVADOR</t>
+          <t>RÍMAC</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
@@ -3052,16 +3052,16 @@
         </is>
       </c>
       <c r="H44" t="n">
-        <v>500</v>
+        <v>1000</v>
       </c>
       <c r="I44" t="inlineStr">
         <is>
-          <t>40002047</t>
+          <t>40002049</t>
         </is>
       </c>
       <c r="J44" t="inlineStr">
         <is>
-          <t>PRIMAX GASOHOL 95</t>
+          <t>EXELON NITRO GASOHOL 95</t>
         </is>
       </c>
       <c r="K44" t="inlineStr">
@@ -3078,32 +3078,32 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>4501031944</t>
+          <t>4501031960</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>P125</t>
+          <t>P201</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>E/S LOLESA</t>
+          <t>E/S CHANCAY 1</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>Av. Francisco Pizarro Cdra. 9, Rímac 15094</t>
+          <t>Av. Panamericana Nte. 90.5, 15130</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>RÍMAC</t>
+          <t>CHANCAY</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>LIMA</t>
+          <t>HUARAL</t>
         </is>
       </c>
       <c r="G45" t="inlineStr">
@@ -3112,16 +3112,16 @@
         </is>
       </c>
       <c r="H45" t="n">
-        <v>2000</v>
+        <v>3000</v>
       </c>
       <c r="I45" t="inlineStr">
         <is>
-          <t>40002023</t>
+          <t>40002019</t>
         </is>
       </c>
       <c r="J45" t="inlineStr">
         <is>
-          <t>ENDURA DIESEL B5 S50 UV</t>
+          <t>MAX-D DIESEL B5 S50 UV</t>
         </is>
       </c>
       <c r="K45" t="inlineStr">
@@ -3138,32 +3138,32 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>4501031945</t>
+          <t>4501031958</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>P125</t>
+          <t>P154</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>E/S LOLESA</t>
+          <t>E/S CHANCAY 2</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>Av. Francisco Pizarro Cdra. 9, Rímac 15094</t>
+          <t>Av. Panamericana Nte. 83.9, 15130</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>RÍMAC</t>
+          <t>CHANCAY</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>LIMA</t>
+          <t>HUARAL</t>
         </is>
       </c>
       <c r="G46" t="inlineStr">
@@ -3172,16 +3172,16 @@
         </is>
       </c>
       <c r="H46" t="n">
-        <v>1000</v>
+        <v>6000</v>
       </c>
       <c r="I46" t="inlineStr">
         <is>
-          <t>40002041</t>
+          <t>40002019</t>
         </is>
       </c>
       <c r="J46" t="inlineStr">
         <is>
-          <t>EXELON GASOHOL 90</t>
+          <t>MAX-D DIESEL B5 S50 UV</t>
         </is>
       </c>
       <c r="K46" t="inlineStr">
@@ -3198,27 +3198,27 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>4501031945</t>
+          <t>4501031969</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>P125</t>
+          <t>P246</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>E/S LOLESA</t>
+          <t>E/S LA PAZ 1</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>Av. Francisco Pizarro Cdra. 9, Rímac 15094</t>
+          <t>Av. La Paz 925, San Miguel 15087</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>RÍMAC</t>
+          <t>SAN MIGUEL</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
@@ -3232,16 +3232,16 @@
         </is>
       </c>
       <c r="H47" t="n">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="I47" t="inlineStr">
         <is>
-          <t>40002049</t>
+          <t>40002019</t>
         </is>
       </c>
       <c r="J47" t="inlineStr">
         <is>
-          <t>EXELON NITRO GASOHOL 95</t>
+          <t>MAX-D DIESEL B5 S50 UV</t>
         </is>
       </c>
       <c r="K47" t="inlineStr">
@@ -3258,32 +3258,32 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>4501031960</t>
+          <t>4501031970</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>P201</t>
+          <t>P246</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>E/S CHANCAY 1</t>
+          <t>E/S LA PAZ 1</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>Av. Panamericana Nte. 90.5, 15130</t>
+          <t>Av. La Paz 925, San Miguel 15087</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>CHANCAY</t>
+          <t>SAN MIGUEL</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>HUARAL</t>
+          <t>LIMA</t>
         </is>
       </c>
       <c r="G48" t="inlineStr">
@@ -3292,16 +3292,16 @@
         </is>
       </c>
       <c r="H48" t="n">
-        <v>3000</v>
+        <v>1000</v>
       </c>
       <c r="I48" t="inlineStr">
         <is>
-          <t>40002019</t>
+          <t>40002039</t>
         </is>
       </c>
       <c r="J48" t="inlineStr">
         <is>
-          <t>MAX-D DIESEL B5 S50 UV</t>
+          <t>PRIMAX GASOHOL 90</t>
         </is>
       </c>
       <c r="K48" t="inlineStr">
@@ -3318,32 +3318,32 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>4501031958</t>
+          <t>4501031970</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>P154</t>
+          <t>P246</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>E/S CHANCAY 2</t>
+          <t>E/S LA PAZ 1</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>Av. Panamericana Nte. 83.9, 15130</t>
+          <t>Av. La Paz 925, San Miguel 15087</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>CHANCAY</t>
+          <t>SAN MIGUEL</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>HUARAL</t>
+          <t>LIMA</t>
         </is>
       </c>
       <c r="G49" t="inlineStr">
@@ -3352,16 +3352,16 @@
         </is>
       </c>
       <c r="H49" t="n">
-        <v>6000</v>
+        <v>1500</v>
       </c>
       <c r="I49" t="inlineStr">
         <is>
-          <t>40002019</t>
+          <t>40002047</t>
         </is>
       </c>
       <c r="J49" t="inlineStr">
         <is>
-          <t>MAX-D DIESEL B5 S50 UV</t>
+          <t>PRIMAX GASOHOL 95</t>
         </is>
       </c>
       <c r="K49" t="inlineStr">
@@ -3378,22 +3378,22 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>4501031969</t>
+          <t>4501031975</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>P246</t>
+          <t>P244</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>E/S LA PAZ 1</t>
+          <t>E/S LA MARINA</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>Av. La Paz 925, San Miguel 15087</t>
+          <t>Av. la Marina 2155, San Miguel 15087</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
@@ -3412,7 +3412,7 @@
         </is>
       </c>
       <c r="H50" t="n">
-        <v>500</v>
+        <v>2000</v>
       </c>
       <c r="I50" t="inlineStr">
         <is>
@@ -3438,27 +3438,27 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>4501031970</t>
+          <t>4501031978</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>P246</t>
+          <t>P132</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>E/S LA PAZ 1</t>
+          <t>E/S TOMÁS VALLE</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>Av. La Paz 925, San Miguel 15087</t>
+          <t>Av. Tomas Valle 846, San Martín de Porres 15302</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>SAN MIGUEL</t>
+          <t>SAN MARTÍN DE PORRES</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
@@ -3476,12 +3476,12 @@
       </c>
       <c r="I51" t="inlineStr">
         <is>
-          <t>40002039</t>
+          <t>40002019</t>
         </is>
       </c>
       <c r="J51" t="inlineStr">
         <is>
-          <t>PRIMAX GASOHOL 90</t>
+          <t>MAX-D DIESEL B5 S50 UV</t>
         </is>
       </c>
       <c r="K51" t="inlineStr">
@@ -3498,27 +3498,27 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>4501031970</t>
+          <t>4501031979</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>P246</t>
+          <t>P132</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>E/S LA PAZ 1</t>
+          <t>E/S TOMÁS VALLE</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>Av. La Paz 925, San Miguel 15087</t>
+          <t>Av. Tomas Valle 846, San Martín de Porres 15302</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>SAN MIGUEL</t>
+          <t>SAN MARTÍN DE PORRES</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
@@ -3532,16 +3532,16 @@
         </is>
       </c>
       <c r="H52" t="n">
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="I52" t="inlineStr">
         <is>
-          <t>40002047</t>
+          <t>40002039</t>
         </is>
       </c>
       <c r="J52" t="inlineStr">
         <is>
-          <t>PRIMAX GASOHOL 95</t>
+          <t>PRIMAX GASOHOL 90</t>
         </is>
       </c>
       <c r="K52" t="inlineStr">
@@ -3558,27 +3558,27 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>4501031975</t>
+          <t>4501031979</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>P244</t>
+          <t>P132</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>E/S LA MARINA</t>
+          <t>E/S TOMÁS VALLE</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>Av. la Marina 2155, San Miguel 15087</t>
+          <t>Av. Tomas Valle 846, San Martín de Porres 15302</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>SAN MIGUEL</t>
+          <t>SAN MARTÍN DE PORRES</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
@@ -3592,16 +3592,16 @@
         </is>
       </c>
       <c r="H53" t="n">
-        <v>2000</v>
+        <v>1000</v>
       </c>
       <c r="I53" t="inlineStr">
         <is>
-          <t>40002019</t>
+          <t>40002047</t>
         </is>
       </c>
       <c r="J53" t="inlineStr">
         <is>
-          <t>MAX-D DIESEL B5 S50 UV</t>
+          <t>PRIMAX GASOHOL 95</t>
         </is>
       </c>
       <c r="K53" t="inlineStr">
@@ -3618,27 +3618,27 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>4501031978</t>
+          <t>4501031981</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>P132</t>
+          <t>P122</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>E/S TOMÁS VALLE</t>
+          <t>E/S ALEGRÍA</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>Av. Tomas Valle 846, San Martín de Porres 15302</t>
+          <t>Av. Alfredo Benavides 2116, Miraflores 15048</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>SAN MARTÍN DE PORRES</t>
+          <t>MIRAFLORES</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
@@ -3678,32 +3678,32 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>4501031979</t>
+          <t>4501031983</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>P132</t>
+          <t>P113</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>E/S TOMÁS VALLE</t>
+          <t>E/S HUARALINO</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>Av. Tomas Valle 846, San Martín de Porres 15302</t>
+          <t>Chancay 351, Huaral 15202</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>SAN MARTÍN DE PORRES</t>
+          <t>HUARAL</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
         <is>
-          <t>LIMA</t>
+          <t>HUARAL</t>
         </is>
       </c>
       <c r="G55" t="inlineStr">
@@ -3712,16 +3712,16 @@
         </is>
       </c>
       <c r="H55" t="n">
-        <v>1000</v>
+        <v>2500</v>
       </c>
       <c r="I55" t="inlineStr">
         <is>
-          <t>40002039</t>
+          <t>40002019</t>
         </is>
       </c>
       <c r="J55" t="inlineStr">
         <is>
-          <t>PRIMAX GASOHOL 90</t>
+          <t>MAX-D DIESEL B5 S50 UV</t>
         </is>
       </c>
       <c r="K55" t="inlineStr">
@@ -3738,32 +3738,32 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>4501031979</t>
+          <t>4501031984</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>P132</t>
+          <t>P113</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>E/S TOMÁS VALLE</t>
+          <t>E/S HUARALINO</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>Av. Tomas Valle 846, San Martín de Porres 15302</t>
+          <t>Chancay 351, Huaral 15202</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>SAN MARTÍN DE PORRES</t>
+          <t>HUARAL</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
         <is>
-          <t>LIMA</t>
+          <t>HUARAL</t>
         </is>
       </c>
       <c r="G56" t="inlineStr">
@@ -3776,12 +3776,12 @@
       </c>
       <c r="I56" t="inlineStr">
         <is>
-          <t>40002047</t>
+          <t>40002039</t>
         </is>
       </c>
       <c r="J56" t="inlineStr">
         <is>
-          <t>PRIMAX GASOHOL 95</t>
+          <t>PRIMAX GASOHOL 90</t>
         </is>
       </c>
       <c r="K56" t="inlineStr">
@@ -3798,32 +3798,32 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>4501031981</t>
+          <t>4501031984</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>P122</t>
+          <t>P113</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>E/S ALEGRÍA</t>
+          <t>E/S HUARALINO</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>Av. Alfredo Benavides 2116, Miraflores 15048</t>
+          <t>Chancay 351, Huaral 15202</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>MIRAFLORES</t>
+          <t>HUARAL</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
         <is>
-          <t>LIMA</t>
+          <t>HUARAL</t>
         </is>
       </c>
       <c r="G57" t="inlineStr">
@@ -3832,16 +3832,16 @@
         </is>
       </c>
       <c r="H57" t="n">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="I57" t="inlineStr">
         <is>
-          <t>40002019</t>
+          <t>40002047</t>
         </is>
       </c>
       <c r="J57" t="inlineStr">
         <is>
-          <t>MAX-D DIESEL B5 S50 UV</t>
+          <t>PRIMAX GASOHOL 95</t>
         </is>
       </c>
       <c r="K57" t="inlineStr">
@@ -3858,32 +3858,32 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>4501031983</t>
+          <t>4501031954</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>P113</t>
+          <t>P159</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>E/S HUARALINO</t>
+          <t>E/S COLONIAL 1</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>Chancay 351, Huaral 15202</t>
+          <t>Ricardo Herrera 1406, Cercado de Lima 15082</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>HUARAL</t>
+          <t>CERCADO DE LIMA</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
         <is>
-          <t>HUARAL</t>
+          <t>LIMA</t>
         </is>
       </c>
       <c r="G58" t="inlineStr">
@@ -3892,7 +3892,7 @@
         </is>
       </c>
       <c r="H58" t="n">
-        <v>2500</v>
+        <v>2000</v>
       </c>
       <c r="I58" t="inlineStr">
         <is>
@@ -3906,44 +3906,44 @@
       </c>
       <c r="K58" t="inlineStr">
         <is>
-          <t>P611</t>
+          <t>P614</t>
         </is>
       </c>
       <c r="L58" t="inlineStr">
         <is>
-          <t>TERMINAL REFINERÍA PAMPILLA</t>
+          <t>TERMINAL PBF CALLAO</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>4501031984</t>
+          <t>4501031956</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>P113</t>
+          <t>P159</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>E/S HUARALINO</t>
+          <t>E/S COLONIAL 1</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>Chancay 351, Huaral 15202</t>
+          <t>Ricardo Herrera 1406, Cercado de Lima 15082</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>HUARAL</t>
+          <t>CERCADO DE LIMA</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
         <is>
-          <t>HUARAL</t>
+          <t>LIMA</t>
         </is>
       </c>
       <c r="G59" t="inlineStr">
@@ -3966,44 +3966,44 @@
       </c>
       <c r="K59" t="inlineStr">
         <is>
-          <t>P611</t>
+          <t>P614</t>
         </is>
       </c>
       <c r="L59" t="inlineStr">
         <is>
-          <t>TERMINAL REFINERÍA PAMPILLA</t>
+          <t>TERMINAL PBF CALLAO</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>4501031984</t>
+          <t>4501031956</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>P113</t>
+          <t>P159</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>E/S HUARALINO</t>
+          <t>E/S COLONIAL 1</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>Chancay 351, Huaral 15202</t>
+          <t>Ricardo Herrera 1406, Cercado de Lima 15082</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>HUARAL</t>
+          <t>CERCADO DE LIMA</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
         <is>
-          <t>HUARAL</t>
+          <t>LIMA</t>
         </is>
       </c>
       <c r="G60" t="inlineStr">
@@ -4026,19 +4026,19 @@
       </c>
       <c r="K60" t="inlineStr">
         <is>
-          <t>P611</t>
+          <t>P614</t>
         </is>
       </c>
       <c r="L60" t="inlineStr">
         <is>
-          <t>TERMINAL REFINERÍA PAMPILLA</t>
+          <t>TERMINAL PBF CALLAO</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>4501031954</t>
+          <t>4501031956</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
@@ -4072,16 +4072,16 @@
         </is>
       </c>
       <c r="H61" t="n">
-        <v>2000</v>
+        <v>500</v>
       </c>
       <c r="I61" t="inlineStr">
         <is>
-          <t>40002019</t>
+          <t>40002055</t>
         </is>
       </c>
       <c r="J61" t="inlineStr">
         <is>
-          <t>MAX-D DIESEL B5 S50 UV</t>
+          <t>G-PRIX GASOHOL 97</t>
         </is>
       </c>
       <c r="K61" t="inlineStr">
@@ -4098,27 +4098,27 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>4501031956</t>
+          <t>4501031946</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>P159</t>
+          <t>P184</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>E/S COLONIAL 1</t>
+          <t>E/S GAMARRA</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>Ricardo Herrera 1406, Cercado de Lima 15082</t>
+          <t>Av. Universitaria 2015, San Martín de Porres 15108</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>CERCADO DE LIMA</t>
+          <t>SAN MARTÍN DE PORRES</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
@@ -4132,16 +4132,16 @@
         </is>
       </c>
       <c r="H62" t="n">
-        <v>1000</v>
+        <v>2000</v>
       </c>
       <c r="I62" t="inlineStr">
         <is>
-          <t>40002039</t>
+          <t>40002023</t>
         </is>
       </c>
       <c r="J62" t="inlineStr">
         <is>
-          <t>PRIMAX GASOHOL 90</t>
+          <t>ENDURA DIESEL B5 S50 UV</t>
         </is>
       </c>
       <c r="K62" t="inlineStr">
@@ -4158,27 +4158,27 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>4501031956</t>
+          <t>4501031947</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>P159</t>
+          <t>P184</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>E/S COLONIAL 1</t>
+          <t>E/S GAMARRA</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>Ricardo Herrera 1406, Cercado de Lima 15082</t>
+          <t>Av. Universitaria 2015, San Martín de Porres 15108</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>CERCADO DE LIMA</t>
+          <t>SAN MARTÍN DE PORRES</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
@@ -4192,16 +4192,16 @@
         </is>
       </c>
       <c r="H63" t="n">
-        <v>500</v>
+        <v>1000</v>
       </c>
       <c r="I63" t="inlineStr">
         <is>
-          <t>40002047</t>
+          <t>40002041</t>
         </is>
       </c>
       <c r="J63" t="inlineStr">
         <is>
-          <t>PRIMAX GASOHOL 95</t>
+          <t>EXELON GASOHOL 90</t>
         </is>
       </c>
       <c r="K63" t="inlineStr">
@@ -4218,27 +4218,27 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>4501031956</t>
+          <t>4501031947</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>P159</t>
+          <t>P184</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>E/S COLONIAL 1</t>
+          <t>E/S GAMARRA</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>Ricardo Herrera 1406, Cercado de Lima 15082</t>
+          <t>Av. Universitaria 2015, San Martín de Porres 15108</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>CERCADO DE LIMA</t>
+          <t>SAN MARTÍN DE PORRES</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
@@ -4256,12 +4256,12 @@
       </c>
       <c r="I64" t="inlineStr">
         <is>
-          <t>40002055</t>
+          <t>40002049</t>
         </is>
       </c>
       <c r="J64" t="inlineStr">
         <is>
-          <t>G-PRIX GASOHOL 97</t>
+          <t>EXELON NITRO GASOHOL 95</t>
         </is>
       </c>
       <c r="K64" t="inlineStr">
@@ -4278,7 +4278,7 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>4501031946</t>
+          <t>4501031947</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
@@ -4312,16 +4312,16 @@
         </is>
       </c>
       <c r="H65" t="n">
-        <v>2000</v>
+        <v>500</v>
       </c>
       <c r="I65" t="inlineStr">
         <is>
-          <t>40002023</t>
+          <t>40002057</t>
         </is>
       </c>
       <c r="J65" t="inlineStr">
         <is>
-          <t>ENDURA DIESEL B5 S50 UV</t>
+          <t>EXELON NITRO GASOHOL 97</t>
         </is>
       </c>
       <c r="K65" t="inlineStr">
@@ -4338,27 +4338,27 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>4501031947</t>
+          <t>4501031948</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>P184</t>
+          <t>P215</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>E/S GAMARRA</t>
+          <t>E/S EL CARMELO</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>Av. Universitaria 2015, San Martín de Porres 15108</t>
+          <t>Av. la Marina 3112, San Miguel 15088</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>SAN MARTÍN DE PORRES</t>
+          <t>SAN MIGUEL</t>
         </is>
       </c>
       <c r="F66" t="inlineStr">
@@ -4372,16 +4372,16 @@
         </is>
       </c>
       <c r="H66" t="n">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="I66" t="inlineStr">
         <is>
-          <t>40002041</t>
+          <t>40002019</t>
         </is>
       </c>
       <c r="J66" t="inlineStr">
         <is>
-          <t>EXELON GASOHOL 90</t>
+          <t>MAX-D DIESEL B5 S50 UV</t>
         </is>
       </c>
       <c r="K66" t="inlineStr">
@@ -4398,27 +4398,27 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>4501031947</t>
+          <t>4501031949</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>P184</t>
+          <t>P215</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>E/S GAMARRA</t>
+          <t>E/S EL CARMELO</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>Av. Universitaria 2015, San Martín de Porres 15108</t>
+          <t>Av. la Marina 3112, San Miguel 15088</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>SAN MARTÍN DE PORRES</t>
+          <t>SAN MIGUEL</t>
         </is>
       </c>
       <c r="F67" t="inlineStr">
@@ -4432,16 +4432,16 @@
         </is>
       </c>
       <c r="H67" t="n">
-        <v>500</v>
+        <v>1000</v>
       </c>
       <c r="I67" t="inlineStr">
         <is>
-          <t>40002049</t>
+          <t>40002039</t>
         </is>
       </c>
       <c r="J67" t="inlineStr">
         <is>
-          <t>EXELON NITRO GASOHOL 95</t>
+          <t>PRIMAX GASOHOL 90</t>
         </is>
       </c>
       <c r="K67" t="inlineStr">
@@ -4458,27 +4458,27 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>4501031947</t>
+          <t>4501031949</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>P184</t>
+          <t>P215</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>E/S GAMARRA</t>
+          <t>E/S EL CARMELO</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>Av. Universitaria 2015, San Martín de Porres 15108</t>
+          <t>Av. la Marina 3112, San Miguel 15088</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>SAN MARTÍN DE PORRES</t>
+          <t>SAN MIGUEL</t>
         </is>
       </c>
       <c r="F68" t="inlineStr">
@@ -4492,16 +4492,16 @@
         </is>
       </c>
       <c r="H68" t="n">
-        <v>500</v>
+        <v>2000</v>
       </c>
       <c r="I68" t="inlineStr">
         <is>
-          <t>40002057</t>
+          <t>40002047</t>
         </is>
       </c>
       <c r="J68" t="inlineStr">
         <is>
-          <t>EXELON NITRO GASOHOL 97</t>
+          <t>PRIMAX GASOHOL 95</t>
         </is>
       </c>
       <c r="K68" t="inlineStr">
@@ -4518,7 +4518,7 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>4501031948</t>
+          <t>4501031949</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
@@ -4556,12 +4556,12 @@
       </c>
       <c r="I69" t="inlineStr">
         <is>
-          <t>40002019</t>
+          <t>40002055</t>
         </is>
       </c>
       <c r="J69" t="inlineStr">
         <is>
-          <t>MAX-D DIESEL B5 S50 UV</t>
+          <t>G-PRIX GASOHOL 97</t>
         </is>
       </c>
       <c r="K69" t="inlineStr">
@@ -4578,27 +4578,27 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>4501031949</t>
+          <t>4501031952</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>P215</t>
+          <t>P236</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>E/S EL CARMELO</t>
+          <t>E/S HUIRACOCHA</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>Av. la Marina 3112, San Miguel 15088</t>
+          <t>Av. Gregorio Escobedo 410, Jesús María 15072</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>SAN MIGUEL</t>
+          <t>JESUS MARIA</t>
         </is>
       </c>
       <c r="F70" t="inlineStr">
@@ -4612,16 +4612,16 @@
         </is>
       </c>
       <c r="H70" t="n">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="I70" t="inlineStr">
         <is>
-          <t>40002039</t>
+          <t>40002019</t>
         </is>
       </c>
       <c r="J70" t="inlineStr">
         <is>
-          <t>PRIMAX GASOHOL 90</t>
+          <t>MAX-D DIESEL B5 S50 UV</t>
         </is>
       </c>
       <c r="K70" t="inlineStr">
@@ -4638,27 +4638,27 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>4501031949</t>
+          <t>4501031953</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>P215</t>
+          <t>P236</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>E/S EL CARMELO</t>
+          <t>E/S HUIRACOCHA</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>Av. la Marina 3112, San Miguel 15088</t>
+          <t>Av. Gregorio Escobedo 410, Jesús María 15072</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>SAN MIGUEL</t>
+          <t>JESUS MARIA</t>
         </is>
       </c>
       <c r="F71" t="inlineStr">
@@ -4672,16 +4672,16 @@
         </is>
       </c>
       <c r="H71" t="n">
-        <v>2000</v>
+        <v>1000</v>
       </c>
       <c r="I71" t="inlineStr">
         <is>
-          <t>40002047</t>
+          <t>40002039</t>
         </is>
       </c>
       <c r="J71" t="inlineStr">
         <is>
-          <t>PRIMAX GASOHOL 95</t>
+          <t>PRIMAX GASOHOL 90</t>
         </is>
       </c>
       <c r="K71" t="inlineStr">
@@ -4698,27 +4698,27 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>4501031949</t>
+          <t>4501031953</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>P215</t>
+          <t>P236</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>E/S EL CARMELO</t>
+          <t>E/S HUIRACOCHA</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>Av. la Marina 3112, San Miguel 15088</t>
+          <t>Av. Gregorio Escobedo 410, Jesús María 15072</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>SAN MIGUEL</t>
+          <t>JESUS MARIA</t>
         </is>
       </c>
       <c r="F72" t="inlineStr">
@@ -4732,16 +4732,16 @@
         </is>
       </c>
       <c r="H72" t="n">
-        <v>500</v>
+        <v>1500</v>
       </c>
       <c r="I72" t="inlineStr">
         <is>
-          <t>40002055</t>
+          <t>40002047</t>
         </is>
       </c>
       <c r="J72" t="inlineStr">
         <is>
-          <t>G-PRIX GASOHOL 97</t>
+          <t>PRIMAX GASOHOL 95</t>
         </is>
       </c>
       <c r="K72" t="inlineStr">
@@ -4758,7 +4758,7 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>4501031952</t>
+          <t>4501031953</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
@@ -4792,16 +4792,16 @@
         </is>
       </c>
       <c r="H73" t="n">
-        <v>500</v>
+        <v>1000</v>
       </c>
       <c r="I73" t="inlineStr">
         <is>
-          <t>40002019</t>
+          <t>40002055</t>
         </is>
       </c>
       <c r="J73" t="inlineStr">
         <is>
-          <t>MAX-D DIESEL B5 S50 UV</t>
+          <t>G-PRIX GASOHOL 97</t>
         </is>
       </c>
       <c r="K73" t="inlineStr">
@@ -4818,27 +4818,27 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>4501031953</t>
+          <t>4501031963</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>P236</t>
+          <t>P199</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>E/S HUIRACOCHA</t>
+          <t>E/S CASTAÑOS</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>Av. Gregorio Escobedo 410, Jesús María 15072</t>
+          <t>Av Javier Prado Oeste 1895, San Isidro 15076</t>
         </is>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>JESUS MARIA</t>
+          <t>SAN ISIDRO</t>
         </is>
       </c>
       <c r="F74" t="inlineStr">
@@ -4852,16 +4852,16 @@
         </is>
       </c>
       <c r="H74" t="n">
-        <v>1000</v>
+        <v>1500</v>
       </c>
       <c r="I74" t="inlineStr">
         <is>
-          <t>40002039</t>
+          <t>40002055</t>
         </is>
       </c>
       <c r="J74" t="inlineStr">
         <is>
-          <t>PRIMAX GASOHOL 90</t>
+          <t>G-PRIX GASOHOL 97</t>
         </is>
       </c>
       <c r="K74" t="inlineStr">
@@ -4878,27 +4878,27 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>4501031953</t>
+          <t>4501031988</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>P236</t>
+          <t>P165</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>E/S HUIRACOCHA</t>
+          <t>E/S ESCARDÓ</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>Av. Gregorio Escobedo 410, Jesús María 15072</t>
+          <t>Av. Rafael Escardó 250, San Miguel 15087</t>
         </is>
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>JESUS MARIA</t>
+          <t>SAN MIGUEL</t>
         </is>
       </c>
       <c r="F75" t="inlineStr">
@@ -4912,16 +4912,16 @@
         </is>
       </c>
       <c r="H75" t="n">
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="I75" t="inlineStr">
         <is>
-          <t>40002047</t>
+          <t>40002019</t>
         </is>
       </c>
       <c r="J75" t="inlineStr">
         <is>
-          <t>PRIMAX GASOHOL 95</t>
+          <t>MAX-D DIESEL B5 S50 UV</t>
         </is>
       </c>
       <c r="K75" t="inlineStr">
@@ -4938,27 +4938,27 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>4501031953</t>
+          <t>4501031989</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>P236</t>
+          <t>P165</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>E/S HUIRACOCHA</t>
+          <t>E/S ESCARDÓ</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>Av. Gregorio Escobedo 410, Jesús María 15072</t>
+          <t>Av. Rafael Escardó 250, San Miguel 15087</t>
         </is>
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>JESUS MARIA</t>
+          <t>SAN MIGUEL</t>
         </is>
       </c>
       <c r="F76" t="inlineStr">
@@ -4972,16 +4972,16 @@
         </is>
       </c>
       <c r="H76" t="n">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="I76" t="inlineStr">
         <is>
-          <t>40002055</t>
+          <t>40002039</t>
         </is>
       </c>
       <c r="J76" t="inlineStr">
         <is>
-          <t>G-PRIX GASOHOL 97</t>
+          <t>PRIMAX GASOHOL 90</t>
         </is>
       </c>
       <c r="K76" t="inlineStr">
@@ -4998,27 +4998,27 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>4501031963</t>
+          <t>4501031989</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>P199</t>
+          <t>P165</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>E/S CASTAÑOS</t>
+          <t>E/S ESCARDÓ</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>Av Javier Prado Oeste 1895, San Isidro 15076</t>
+          <t>Av. Rafael Escardó 250, San Miguel 15087</t>
         </is>
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>SAN ISIDRO</t>
+          <t>SAN MIGUEL</t>
         </is>
       </c>
       <c r="F77" t="inlineStr">
@@ -5032,7 +5032,7 @@
         </is>
       </c>
       <c r="H77" t="n">
-        <v>1500</v>
+        <v>500</v>
       </c>
       <c r="I77" t="inlineStr">
         <is>
@@ -5058,27 +5058,27 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>4501031988</t>
+          <t>4501031990</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>P165</t>
+          <t>P167</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>E/S ESCARDÓ</t>
+          <t>E/S MIRAFLORES</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>Av. Rafael Escardó 250, San Miguel 15087</t>
+          <t>VXGG+H2W, Lima 15074</t>
         </is>
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>SAN MIGUEL</t>
+          <t>MIRAFLORES</t>
         </is>
       </c>
       <c r="F78" t="inlineStr">
@@ -5092,16 +5092,16 @@
         </is>
       </c>
       <c r="H78" t="n">
-        <v>1000</v>
+        <v>2000</v>
       </c>
       <c r="I78" t="inlineStr">
         <is>
-          <t>40002019</t>
+          <t>40002047</t>
         </is>
       </c>
       <c r="J78" t="inlineStr">
         <is>
-          <t>MAX-D DIESEL B5 S50 UV</t>
+          <t>PRIMAX GASOHOL 95</t>
         </is>
       </c>
       <c r="K78" t="inlineStr">
@@ -5118,27 +5118,27 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>4501031989</t>
+          <t>4501031990</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>P165</t>
+          <t>P167</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>E/S ESCARDÓ</t>
+          <t>E/S MIRAFLORES</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>Av. Rafael Escardó 250, San Miguel 15087</t>
+          <t>VXGG+H2W, Lima 15074</t>
         </is>
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>SAN MIGUEL</t>
+          <t>MIRAFLORES</t>
         </is>
       </c>
       <c r="F79" t="inlineStr">
@@ -5156,12 +5156,12 @@
       </c>
       <c r="I79" t="inlineStr">
         <is>
-          <t>40002039</t>
+          <t>40002055</t>
         </is>
       </c>
       <c r="J79" t="inlineStr">
         <is>
-          <t>PRIMAX GASOHOL 90</t>
+          <t>G-PRIX GASOHOL 97</t>
         </is>
       </c>
       <c r="K79" t="inlineStr">
@@ -5178,27 +5178,27 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>4501031989</t>
+          <t>4501031991</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>P165</t>
+          <t>P309</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>E/S ESCARDÓ</t>
+          <t>E/S SUDAMERICANO</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>Av. Rafael Escardó 250, San Miguel 15087</t>
+          <t>Av. Tingo Maria, Cercado de Lima 15082</t>
         </is>
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>SAN MIGUEL</t>
+          <t>CERCADO DE LIMA</t>
         </is>
       </c>
       <c r="F80" t="inlineStr">
@@ -5212,16 +5212,16 @@
         </is>
       </c>
       <c r="H80" t="n">
-        <v>500</v>
+        <v>1000</v>
       </c>
       <c r="I80" t="inlineStr">
         <is>
-          <t>40002055</t>
+          <t>40002039</t>
         </is>
       </c>
       <c r="J80" t="inlineStr">
         <is>
-          <t>G-PRIX GASOHOL 97</t>
+          <t>PRIMAX GASOHOL 90</t>
         </is>
       </c>
       <c r="K80" t="inlineStr">
@@ -5238,27 +5238,27 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>4501031990</t>
+          <t>4501031991</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>P167</t>
+          <t>P309</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>E/S MIRAFLORES</t>
+          <t>E/S SUDAMERICANO</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>VXGG+H2W, Lima 15074</t>
+          <t>Av. Tingo Maria, Cercado de Lima 15082</t>
         </is>
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>MIRAFLORES</t>
+          <t>CERCADO DE LIMA</t>
         </is>
       </c>
       <c r="F81" t="inlineStr">
@@ -5272,7 +5272,7 @@
         </is>
       </c>
       <c r="H81" t="n">
-        <v>2000</v>
+        <v>2500</v>
       </c>
       <c r="I81" t="inlineStr">
         <is>
@@ -5298,27 +5298,27 @@
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>4501031990</t>
+          <t>4501031991</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>P167</t>
+          <t>P309</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>E/S MIRAFLORES</t>
+          <t>E/S SUDAMERICANO</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>VXGG+H2W, Lima 15074</t>
+          <t>Av. Tingo Maria, Cercado de Lima 15082</t>
         </is>
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>MIRAFLORES</t>
+          <t>CERCADO DE LIMA</t>
         </is>
       </c>
       <c r="F82" t="inlineStr">
@@ -5332,7 +5332,7 @@
         </is>
       </c>
       <c r="H82" t="n">
-        <v>500</v>
+        <v>1000</v>
       </c>
       <c r="I82" t="inlineStr">
         <is>
@@ -5358,32 +5358,32 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>4501031991</t>
+          <t>4501031993</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>P309</t>
+          <t>P194</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>E/S SUDAMERICANO</t>
+          <t>E/S CALLE DERECHA</t>
         </is>
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>Av. Tingo Maria, Cercado de Lima 15082</t>
+          <t>Av García Alonso 195, Huaral 15201</t>
         </is>
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>CERCADO DE LIMA</t>
+          <t>HUARAL</t>
         </is>
       </c>
       <c r="F83" t="inlineStr">
         <is>
-          <t>LIMA</t>
+          <t>HUARAL</t>
         </is>
       </c>
       <c r="G83" t="inlineStr">
@@ -5392,58 +5392,58 @@
         </is>
       </c>
       <c r="H83" t="n">
-        <v>1000</v>
+        <v>2000</v>
       </c>
       <c r="I83" t="inlineStr">
         <is>
-          <t>40002039</t>
+          <t>40002019</t>
         </is>
       </c>
       <c r="J83" t="inlineStr">
         <is>
-          <t>PRIMAX GASOHOL 90</t>
+          <t>MAX-D DIESEL B5 S50 UV</t>
         </is>
       </c>
       <c r="K83" t="inlineStr">
         <is>
-          <t>P614</t>
+          <t>P611</t>
         </is>
       </c>
       <c r="L83" t="inlineStr">
         <is>
-          <t>TERMINAL PBF CALLAO</t>
+          <t>TERMINAL REFINERÍA PAMPILLA</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>4501031991</t>
+          <t>4501031994</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>P309</t>
+          <t>P194</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>E/S SUDAMERICANO</t>
+          <t>E/S CALLE DERECHA</t>
         </is>
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>Av. Tingo Maria, Cercado de Lima 15082</t>
+          <t>Av García Alonso 195, Huaral 15201</t>
         </is>
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>CERCADO DE LIMA</t>
+          <t>HUARAL</t>
         </is>
       </c>
       <c r="F84" t="inlineStr">
         <is>
-          <t>LIMA</t>
+          <t>HUARAL</t>
         </is>
       </c>
       <c r="G84" t="inlineStr">
@@ -5452,58 +5452,58 @@
         </is>
       </c>
       <c r="H84" t="n">
-        <v>2500</v>
+        <v>3250</v>
       </c>
       <c r="I84" t="inlineStr">
         <is>
-          <t>40002047</t>
+          <t>40002039</t>
         </is>
       </c>
       <c r="J84" t="inlineStr">
         <is>
-          <t>PRIMAX GASOHOL 95</t>
+          <t>PRIMAX GASOHOL 90</t>
         </is>
       </c>
       <c r="K84" t="inlineStr">
         <is>
-          <t>P614</t>
+          <t>P611</t>
         </is>
       </c>
       <c r="L84" t="inlineStr">
         <is>
-          <t>TERMINAL PBF CALLAO</t>
+          <t>TERMINAL REFINERÍA PAMPILLA</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>4501031991</t>
+          <t>4501031994</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>P309</t>
+          <t>P194</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>E/S SUDAMERICANO</t>
+          <t>E/S CALLE DERECHA</t>
         </is>
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>Av. Tingo Maria, Cercado de Lima 15082</t>
+          <t>Av García Alonso 195, Huaral 15201</t>
         </is>
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>CERCADO DE LIMA</t>
+          <t>HUARAL</t>
         </is>
       </c>
       <c r="F85" t="inlineStr">
         <is>
-          <t>LIMA</t>
+          <t>HUARAL</t>
         </is>
       </c>
       <c r="G85" t="inlineStr">
@@ -5512,58 +5512,58 @@
         </is>
       </c>
       <c r="H85" t="n">
-        <v>1000</v>
+        <v>750</v>
       </c>
       <c r="I85" t="inlineStr">
         <is>
-          <t>40002055</t>
+          <t>40002047</t>
         </is>
       </c>
       <c r="J85" t="inlineStr">
         <is>
-          <t>G-PRIX GASOHOL 97</t>
+          <t>PRIMAX GASOHOL 95</t>
         </is>
       </c>
       <c r="K85" t="inlineStr">
         <is>
-          <t>P614</t>
+          <t>P611</t>
         </is>
       </c>
       <c r="L85" t="inlineStr">
         <is>
-          <t>TERMINAL PBF CALLAO</t>
+          <t>TERMINAL REFINERÍA PAMPILLA</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>4501031993</t>
+          <t>4501031995</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>P194</t>
+          <t>P294</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>E/S CALLE DERECHA</t>
+          <t>E/S SAN JOSÉ</t>
         </is>
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>Av García Alonso 195, Huaral 15201</t>
+          <t>Av. Panamericana Nte. 928, Barranca 15169</t>
         </is>
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>HUARAL</t>
+          <t>BARRANCA</t>
         </is>
       </c>
       <c r="F86" t="inlineStr">
         <is>
-          <t>HUARAL</t>
+          <t>BARRANCA</t>
         </is>
       </c>
       <c r="G86" t="inlineStr">
@@ -5572,7 +5572,7 @@
         </is>
       </c>
       <c r="H86" t="n">
-        <v>2000</v>
+        <v>3000</v>
       </c>
       <c r="I86" t="inlineStr">
         <is>
@@ -5598,32 +5598,32 @@
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>4501031994</t>
+          <t>4501031997</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>P194</t>
+          <t>P244</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>E/S CALLE DERECHA</t>
+          <t>E/S LA MARINA</t>
         </is>
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>Av García Alonso 195, Huaral 15201</t>
+          <t>Av. la Marina 2155, San Miguel 15087</t>
         </is>
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>HUARAL</t>
+          <t>SAN MIGUEL</t>
         </is>
       </c>
       <c r="F87" t="inlineStr">
         <is>
-          <t>HUARAL</t>
+          <t>LIMA</t>
         </is>
       </c>
       <c r="G87" t="inlineStr">
@@ -5632,7 +5632,7 @@
         </is>
       </c>
       <c r="H87" t="n">
-        <v>3250</v>
+        <v>1000</v>
       </c>
       <c r="I87" t="inlineStr">
         <is>
@@ -5658,32 +5658,32 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>4501031994</t>
+          <t>4501031997</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>P194</t>
+          <t>P244</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>E/S CALLE DERECHA</t>
+          <t>E/S LA MARINA</t>
         </is>
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>Av García Alonso 195, Huaral 15201</t>
+          <t>Av. la Marina 2155, San Miguel 15087</t>
         </is>
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t>HUARAL</t>
+          <t>SAN MIGUEL</t>
         </is>
       </c>
       <c r="F88" t="inlineStr">
         <is>
-          <t>HUARAL</t>
+          <t>LIMA</t>
         </is>
       </c>
       <c r="G88" t="inlineStr">
@@ -5692,7 +5692,7 @@
         </is>
       </c>
       <c r="H88" t="n">
-        <v>750</v>
+        <v>1000</v>
       </c>
       <c r="I88" t="inlineStr">
         <is>
@@ -5718,32 +5718,32 @@
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>4501031995</t>
+          <t>4501031904</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>P294</t>
+          <t>P135</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>E/S SAN JOSÉ</t>
+          <t>E/S ATE 1</t>
         </is>
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>Av. Panamericana Nte. 928, Barranca 15169</t>
+          <t>Tomas Alva Edison 160, Lima 15022</t>
         </is>
       </c>
       <c r="E89" t="inlineStr">
         <is>
-          <t>BARRANCA</t>
+          <t>ATE</t>
         </is>
       </c>
       <c r="F89" t="inlineStr">
         <is>
-          <t>BARRANCA</t>
+          <t>LIMA</t>
         </is>
       </c>
       <c r="G89" t="inlineStr">
@@ -5752,7 +5752,7 @@
         </is>
       </c>
       <c r="H89" t="n">
-        <v>3000</v>
+        <v>2000</v>
       </c>
       <c r="I89" t="inlineStr">
         <is>
@@ -5778,27 +5778,27 @@
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>4501031997</t>
+          <t>4501031906</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>P244</t>
+          <t>P135</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>E/S LA MARINA</t>
+          <t>E/S ATE 1</t>
         </is>
       </c>
       <c r="D90" t="inlineStr">
         <is>
-          <t>Av. la Marina 2155, San Miguel 15087</t>
+          <t>Tomas Alva Edison 160, Lima 15022</t>
         </is>
       </c>
       <c r="E90" t="inlineStr">
         <is>
-          <t>SAN MIGUEL</t>
+          <t>ATE</t>
         </is>
       </c>
       <c r="F90" t="inlineStr">
@@ -5812,7 +5812,7 @@
         </is>
       </c>
       <c r="H90" t="n">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="I90" t="inlineStr">
         <is>
@@ -5838,27 +5838,27 @@
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>4501031997</t>
+          <t>4501032008</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>P244</t>
+          <t>P296</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>E/S LA MARINA</t>
+          <t>E/S SAN LUIS 1</t>
         </is>
       </c>
       <c r="D91" t="inlineStr">
         <is>
-          <t>Av. la Marina 2155, San Miguel 15087</t>
+          <t>Av. Nicolás Ayllón 1340, San Luis 15019</t>
         </is>
       </c>
       <c r="E91" t="inlineStr">
         <is>
-          <t>SAN MIGUEL</t>
+          <t>SAN LUIS</t>
         </is>
       </c>
       <c r="F91" t="inlineStr">
@@ -5872,16 +5872,16 @@
         </is>
       </c>
       <c r="H91" t="n">
-        <v>1000</v>
+        <v>3000</v>
       </c>
       <c r="I91" t="inlineStr">
         <is>
-          <t>40002047</t>
+          <t>40002019</t>
         </is>
       </c>
       <c r="J91" t="inlineStr">
         <is>
-          <t>PRIMAX GASOHOL 95</t>
+          <t>MAX-D DIESEL B5 S50 UV</t>
         </is>
       </c>
       <c r="K91" t="inlineStr">
@@ -5898,27 +5898,27 @@
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>4501031904</t>
+          <t>4501032009</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>P135</t>
+          <t>P296</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>E/S ATE 1</t>
+          <t>E/S SAN LUIS 1</t>
         </is>
       </c>
       <c r="D92" t="inlineStr">
         <is>
-          <t>Tomas Alva Edison 160, Lima 15022</t>
+          <t>Av. Nicolás Ayllón 1340, San Luis 15019</t>
         </is>
       </c>
       <c r="E92" t="inlineStr">
         <is>
-          <t>ATE</t>
+          <t>SAN LUIS</t>
         </is>
       </c>
       <c r="F92" t="inlineStr">
@@ -5932,16 +5932,16 @@
         </is>
       </c>
       <c r="H92" t="n">
-        <v>2000</v>
+        <v>1000</v>
       </c>
       <c r="I92" t="inlineStr">
         <is>
-          <t>40002019</t>
+          <t>40002039</t>
         </is>
       </c>
       <c r="J92" t="inlineStr">
         <is>
-          <t>MAX-D DIESEL B5 S50 UV</t>
+          <t>PRIMAX GASOHOL 90</t>
         </is>
       </c>
       <c r="K92" t="inlineStr">
@@ -5958,27 +5958,27 @@
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>4501031906</t>
+          <t>4501032016</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>P135</t>
+          <t>P162</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>E/S ATE 1</t>
+          <t>E/S TOMÁS MARSANO</t>
         </is>
       </c>
       <c r="D93" t="inlineStr">
         <is>
-          <t>Tomas Alva Edison 160, Lima 15022</t>
+          <t>Av Tomás Marsano 4080, Santiago de Surco 15039</t>
         </is>
       </c>
       <c r="E93" t="inlineStr">
         <is>
-          <t>ATE</t>
+          <t>SANTIAGO DE SURCO</t>
         </is>
       </c>
       <c r="F93" t="inlineStr">
@@ -5996,49 +5996,49 @@
       </c>
       <c r="I93" t="inlineStr">
         <is>
-          <t>40002039</t>
+          <t>40002019</t>
         </is>
       </c>
       <c r="J93" t="inlineStr">
         <is>
-          <t>PRIMAX GASOHOL 90</t>
+          <t>MAX-D DIESEL B5 S50 UV</t>
         </is>
       </c>
       <c r="K93" t="inlineStr">
         <is>
-          <t>P611</t>
+          <t>P601</t>
         </is>
       </c>
       <c r="L93" t="inlineStr">
         <is>
-          <t>TERMINAL REFINERÍA PAMPILLA</t>
+          <t>TERMINAL REFINERÍA CONCHÁN</t>
         </is>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>4501032008</t>
+          <t>4501032017</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>P296</t>
+          <t>P162</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>E/S SAN LUIS 1</t>
+          <t>E/S TOMÁS MARSANO</t>
         </is>
       </c>
       <c r="D94" t="inlineStr">
         <is>
-          <t>Av. Nicolás Ayllón 1340, San Luis 15019</t>
+          <t>Av Tomás Marsano 4080, Santiago de Surco 15039</t>
         </is>
       </c>
       <c r="E94" t="inlineStr">
         <is>
-          <t>SAN LUIS</t>
+          <t>SANTIAGO DE SURCO</t>
         </is>
       </c>
       <c r="F94" t="inlineStr">
@@ -6052,53 +6052,53 @@
         </is>
       </c>
       <c r="H94" t="n">
-        <v>3000</v>
+        <v>1000</v>
       </c>
       <c r="I94" t="inlineStr">
         <is>
-          <t>40002019</t>
+          <t>40002039</t>
         </is>
       </c>
       <c r="J94" t="inlineStr">
         <is>
-          <t>MAX-D DIESEL B5 S50 UV</t>
+          <t>PRIMAX GASOHOL 90</t>
         </is>
       </c>
       <c r="K94" t="inlineStr">
         <is>
-          <t>P611</t>
+          <t>P601</t>
         </is>
       </c>
       <c r="L94" t="inlineStr">
         <is>
-          <t>TERMINAL REFINERÍA PAMPILLA</t>
+          <t>TERMINAL REFINERÍA CONCHÁN</t>
         </is>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>4501032009</t>
+          <t>4501032017</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>P296</t>
+          <t>P162</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>E/S SAN LUIS 1</t>
+          <t>E/S TOMÁS MARSANO</t>
         </is>
       </c>
       <c r="D95" t="inlineStr">
         <is>
-          <t>Av. Nicolás Ayllón 1340, San Luis 15019</t>
+          <t>Av Tomás Marsano 4080, Santiago de Surco 15039</t>
         </is>
       </c>
       <c r="E95" t="inlineStr">
         <is>
-          <t>SAN LUIS</t>
+          <t>SANTIAGO DE SURCO</t>
         </is>
       </c>
       <c r="F95" t="inlineStr">
@@ -6112,33 +6112,33 @@
         </is>
       </c>
       <c r="H95" t="n">
-        <v>1000</v>
+        <v>2000</v>
       </c>
       <c r="I95" t="inlineStr">
         <is>
-          <t>40002039</t>
+          <t>40002047</t>
         </is>
       </c>
       <c r="J95" t="inlineStr">
         <is>
-          <t>PRIMAX GASOHOL 90</t>
+          <t>PRIMAX GASOHOL 95</t>
         </is>
       </c>
       <c r="K95" t="inlineStr">
         <is>
-          <t>P611</t>
+          <t>P601</t>
         </is>
       </c>
       <c r="L95" t="inlineStr">
         <is>
-          <t>TERMINAL REFINERÍA PAMPILLA</t>
+          <t>TERMINAL REFINERÍA CONCHÁN</t>
         </is>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>4501032016</t>
+          <t>4501032017</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
@@ -6176,12 +6176,12 @@
       </c>
       <c r="I96" t="inlineStr">
         <is>
-          <t>40002019</t>
+          <t>40002055</t>
         </is>
       </c>
       <c r="J96" t="inlineStr">
         <is>
-          <t>MAX-D DIESEL B5 S50 UV</t>
+          <t>G-PRIX GASOHOL 97</t>
         </is>
       </c>
       <c r="K96" t="inlineStr">
@@ -6198,27 +6198,27 @@
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>4501032017</t>
+          <t>4501032015</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>P162</t>
+          <t>P152</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>E/S TOMÁS MARSANO</t>
+          <t>E/S NAVAL</t>
         </is>
       </c>
       <c r="D97" t="inlineStr">
         <is>
-          <t>Av Tomás Marsano 4080, Santiago de Surco 15039</t>
+          <t>Av. San Luis 2480, San Borja 15037</t>
         </is>
       </c>
       <c r="E97" t="inlineStr">
         <is>
-          <t>SANTIAGO DE SURCO</t>
+          <t>SAN BORJA</t>
         </is>
       </c>
       <c r="F97" t="inlineStr">
@@ -6258,27 +6258,27 @@
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>4501032017</t>
+          <t>4501032015</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>P162</t>
+          <t>P152</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>E/S TOMÁS MARSANO</t>
+          <t>E/S NAVAL</t>
         </is>
       </c>
       <c r="D98" t="inlineStr">
         <is>
-          <t>Av Tomás Marsano 4080, Santiago de Surco 15039</t>
+          <t>Av. San Luis 2480, San Borja 15037</t>
         </is>
       </c>
       <c r="E98" t="inlineStr">
         <is>
-          <t>SANTIAGO DE SURCO</t>
+          <t>SAN BORJA</t>
         </is>
       </c>
       <c r="F98" t="inlineStr">
@@ -6318,27 +6318,27 @@
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>4501032017</t>
+          <t>4501032015</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>P162</t>
+          <t>P152</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>E/S TOMÁS MARSANO</t>
+          <t>E/S NAVAL</t>
         </is>
       </c>
       <c r="D99" t="inlineStr">
         <is>
-          <t>Av Tomás Marsano 4080, Santiago de Surco 15039</t>
+          <t>Av. San Luis 2480, San Borja 15037</t>
         </is>
       </c>
       <c r="E99" t="inlineStr">
         <is>
-          <t>SANTIAGO DE SURCO</t>
+          <t>SAN BORJA</t>
         </is>
       </c>
       <c r="F99" t="inlineStr">
@@ -6352,7 +6352,7 @@
         </is>
       </c>
       <c r="H99" t="n">
-        <v>500</v>
+        <v>1000</v>
       </c>
       <c r="I99" t="inlineStr">
         <is>
@@ -6378,27 +6378,27 @@
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>4501032015</t>
+          <t>4501032018</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>P152</t>
+          <t>P216</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>E/S NAVAL</t>
+          <t>E/S EL CHORRILLANO</t>
         </is>
       </c>
       <c r="D100" t="inlineStr">
         <is>
-          <t>Av. San Luis 2480, San Borja 15037</t>
+          <t>Av. Defensores del Morro 350, Cercado de Lima, 15064</t>
         </is>
       </c>
       <c r="E100" t="inlineStr">
         <is>
-          <t>SAN BORJA</t>
+          <t>CHORRILLOS</t>
         </is>
       </c>
       <c r="F100" t="inlineStr">
@@ -6412,16 +6412,16 @@
         </is>
       </c>
       <c r="H100" t="n">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="I100" t="inlineStr">
         <is>
-          <t>40002039</t>
+          <t>40002019</t>
         </is>
       </c>
       <c r="J100" t="inlineStr">
         <is>
-          <t>PRIMAX GASOHOL 90</t>
+          <t>MAX-D DIESEL B5 S50 UV</t>
         </is>
       </c>
       <c r="K100" t="inlineStr">
@@ -6438,27 +6438,27 @@
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>4501032015</t>
+          <t>4501032019</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>P152</t>
+          <t>P216</t>
         </is>
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>E/S NAVAL</t>
+          <t>E/S EL CHORRILLANO</t>
         </is>
       </c>
       <c r="D101" t="inlineStr">
         <is>
-          <t>Av. San Luis 2480, San Borja 15037</t>
+          <t>Av. Defensores del Morro 350, Cercado de Lima, 15064</t>
         </is>
       </c>
       <c r="E101" t="inlineStr">
         <is>
-          <t>SAN BORJA</t>
+          <t>CHORRILLOS</t>
         </is>
       </c>
       <c r="F101" t="inlineStr">
@@ -6476,12 +6476,12 @@
       </c>
       <c r="I101" t="inlineStr">
         <is>
-          <t>40002047</t>
+          <t>40002039</t>
         </is>
       </c>
       <c r="J101" t="inlineStr">
         <is>
-          <t>PRIMAX GASOHOL 95</t>
+          <t>PRIMAX GASOHOL 90</t>
         </is>
       </c>
       <c r="K101" t="inlineStr">
@@ -6498,27 +6498,27 @@
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>4501032015</t>
+          <t>4501032019</t>
         </is>
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>P152</t>
+          <t>P216</t>
         </is>
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>E/S NAVAL</t>
+          <t>E/S EL CHORRILLANO</t>
         </is>
       </c>
       <c r="D102" t="inlineStr">
         <is>
-          <t>Av. San Luis 2480, San Borja 15037</t>
+          <t>Av. Defensores del Morro 350, Cercado de Lima, 15064</t>
         </is>
       </c>
       <c r="E102" t="inlineStr">
         <is>
-          <t>SAN BORJA</t>
+          <t>CHORRILLOS</t>
         </is>
       </c>
       <c r="F102" t="inlineStr">
@@ -6532,16 +6532,16 @@
         </is>
       </c>
       <c r="H102" t="n">
-        <v>1000</v>
+        <v>2500</v>
       </c>
       <c r="I102" t="inlineStr">
         <is>
-          <t>40002055</t>
+          <t>40002047</t>
         </is>
       </c>
       <c r="J102" t="inlineStr">
         <is>
-          <t>G-PRIX GASOHOL 97</t>
+          <t>PRIMAX GASOHOL 95</t>
         </is>
       </c>
       <c r="K102" t="inlineStr">
@@ -6558,7 +6558,7 @@
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>4501032018</t>
+          <t>4501032019</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
@@ -6592,16 +6592,16 @@
         </is>
       </c>
       <c r="H103" t="n">
-        <v>500</v>
+        <v>1000</v>
       </c>
       <c r="I103" t="inlineStr">
         <is>
-          <t>40002019</t>
+          <t>40002055</t>
         </is>
       </c>
       <c r="J103" t="inlineStr">
         <is>
-          <t>MAX-D DIESEL B5 S50 UV</t>
+          <t>G-PRIX GASOHOL 97</t>
         </is>
       </c>
       <c r="K103" t="inlineStr">
@@ -6618,27 +6618,27 @@
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>4501032019</t>
+          <t>4501032012</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>P216</t>
+          <t>P102</t>
         </is>
       </c>
       <c r="C104" t="inlineStr">
         <is>
-          <t>E/S EL CHORRILLANO</t>
+          <t>E/S 28 DE JULIO</t>
         </is>
       </c>
       <c r="D104" t="inlineStr">
         <is>
-          <t>Av. Defensores del Morro 350, Cercado de Lima, 15064</t>
+          <t>Avenida 28 de Julio 2200, La Victoria 15018</t>
         </is>
       </c>
       <c r="E104" t="inlineStr">
         <is>
-          <t>CHORRILLOS</t>
+          <t>LA VICTORIA</t>
         </is>
       </c>
       <c r="F104" t="inlineStr">
@@ -6652,53 +6652,53 @@
         </is>
       </c>
       <c r="H104" t="n">
-        <v>2000</v>
+        <v>3000</v>
       </c>
       <c r="I104" t="inlineStr">
         <is>
-          <t>40002039</t>
+          <t>40002019</t>
         </is>
       </c>
       <c r="J104" t="inlineStr">
         <is>
-          <t>PRIMAX GASOHOL 90</t>
+          <t>MAX-D DIESEL B5 S50 UV</t>
         </is>
       </c>
       <c r="K104" t="inlineStr">
         <is>
-          <t>P601</t>
+          <t>P611</t>
         </is>
       </c>
       <c r="L104" t="inlineStr">
         <is>
-          <t>TERMINAL REFINERÍA CONCHÁN</t>
+          <t>TERMINAL REFINERÍA PAMPILLA</t>
         </is>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>4501032019</t>
+          <t>4501032013</t>
         </is>
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>P216</t>
+          <t>P102</t>
         </is>
       </c>
       <c r="C105" t="inlineStr">
         <is>
-          <t>E/S EL CHORRILLANO</t>
+          <t>E/S 28 DE JULIO</t>
         </is>
       </c>
       <c r="D105" t="inlineStr">
         <is>
-          <t>Av. Defensores del Morro 350, Cercado de Lima, 15064</t>
+          <t>Avenida 28 de Julio 2200, La Victoria 15018</t>
         </is>
       </c>
       <c r="E105" t="inlineStr">
         <is>
-          <t>CHORRILLOS</t>
+          <t>LA VICTORIA</t>
         </is>
       </c>
       <c r="F105" t="inlineStr">
@@ -6712,53 +6712,53 @@
         </is>
       </c>
       <c r="H105" t="n">
-        <v>2500</v>
+        <v>500</v>
       </c>
       <c r="I105" t="inlineStr">
         <is>
-          <t>40002047</t>
+          <t>40002039</t>
         </is>
       </c>
       <c r="J105" t="inlineStr">
         <is>
-          <t>PRIMAX GASOHOL 95</t>
+          <t>PRIMAX GASOHOL 90</t>
         </is>
       </c>
       <c r="K105" t="inlineStr">
         <is>
-          <t>P601</t>
+          <t>P611</t>
         </is>
       </c>
       <c r="L105" t="inlineStr">
         <is>
-          <t>TERMINAL REFINERÍA CONCHÁN</t>
+          <t>TERMINAL REFINERÍA PAMPILLA</t>
         </is>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>4501032019</t>
+          <t>4501032013</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>P216</t>
+          <t>P102</t>
         </is>
       </c>
       <c r="C106" t="inlineStr">
         <is>
-          <t>E/S EL CHORRILLANO</t>
+          <t>E/S 28 DE JULIO</t>
         </is>
       </c>
       <c r="D106" t="inlineStr">
         <is>
-          <t>Av. Defensores del Morro 350, Cercado de Lima, 15064</t>
+          <t>Avenida 28 de Julio 2200, La Victoria 15018</t>
         </is>
       </c>
       <c r="E106" t="inlineStr">
         <is>
-          <t>CHORRILLOS</t>
+          <t>LA VICTORIA</t>
         </is>
       </c>
       <c r="F106" t="inlineStr">
@@ -6772,53 +6772,53 @@
         </is>
       </c>
       <c r="H106" t="n">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="I106" t="inlineStr">
         <is>
-          <t>40002055</t>
+          <t>40002047</t>
         </is>
       </c>
       <c r="J106" t="inlineStr">
         <is>
-          <t>G-PRIX GASOHOL 97</t>
+          <t>PRIMAX GASOHOL 95</t>
         </is>
       </c>
       <c r="K106" t="inlineStr">
         <is>
-          <t>P601</t>
+          <t>P611</t>
         </is>
       </c>
       <c r="L106" t="inlineStr">
         <is>
-          <t>TERMINAL REFINERÍA CONCHÁN</t>
+          <t>TERMINAL REFINERÍA PAMPILLA</t>
         </is>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>4501032012</t>
+          <t>4501032010</t>
         </is>
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>P102</t>
+          <t>P171</t>
         </is>
       </c>
       <c r="C107" t="inlineStr">
         <is>
-          <t>E/S 28 DE JULIO</t>
+          <t>E/S WIESSE</t>
         </is>
       </c>
       <c r="D107" t="inlineStr">
         <is>
-          <t>Avenida 28 de Julio 2200, La Victoria 15018</t>
+          <t>Av. El Bosque, San Juan de Lurigancho 15419</t>
         </is>
       </c>
       <c r="E107" t="inlineStr">
         <is>
-          <t>LA VICTORIA</t>
+          <t>CANTO GRANDE</t>
         </is>
       </c>
       <c r="F107" t="inlineStr">
@@ -6832,7 +6832,7 @@
         </is>
       </c>
       <c r="H107" t="n">
-        <v>3000</v>
+        <v>2000</v>
       </c>
       <c r="I107" t="inlineStr">
         <is>
@@ -6858,27 +6858,27 @@
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>4501032013</t>
+          <t>4501032011</t>
         </is>
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>P102</t>
+          <t>P171</t>
         </is>
       </c>
       <c r="C108" t="inlineStr">
         <is>
-          <t>E/S 28 DE JULIO</t>
+          <t>E/S WIESSE</t>
         </is>
       </c>
       <c r="D108" t="inlineStr">
         <is>
-          <t>Avenida 28 de Julio 2200, La Victoria 15018</t>
+          <t>Av. El Bosque, San Juan de Lurigancho 15419</t>
         </is>
       </c>
       <c r="E108" t="inlineStr">
         <is>
-          <t>LA VICTORIA</t>
+          <t>CANTO GRANDE</t>
         </is>
       </c>
       <c r="F108" t="inlineStr">
@@ -6892,7 +6892,7 @@
         </is>
       </c>
       <c r="H108" t="n">
-        <v>500</v>
+        <v>1000</v>
       </c>
       <c r="I108" t="inlineStr">
         <is>
@@ -6918,27 +6918,27 @@
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>4501032013</t>
+          <t>4501032011</t>
         </is>
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>P102</t>
+          <t>P171</t>
         </is>
       </c>
       <c r="C109" t="inlineStr">
         <is>
-          <t>E/S 28 DE JULIO</t>
+          <t>E/S WIESSE</t>
         </is>
       </c>
       <c r="D109" t="inlineStr">
         <is>
-          <t>Avenida 28 de Julio 2200, La Victoria 15018</t>
+          <t>Av. El Bosque, San Juan de Lurigancho 15419</t>
         </is>
       </c>
       <c r="E109" t="inlineStr">
         <is>
-          <t>LA VICTORIA</t>
+          <t>CANTO GRANDE</t>
         </is>
       </c>
       <c r="F109" t="inlineStr">
@@ -6952,7 +6952,7 @@
         </is>
       </c>
       <c r="H109" t="n">
-        <v>500</v>
+        <v>1000</v>
       </c>
       <c r="I109" t="inlineStr">
         <is>
@@ -6978,27 +6978,27 @@
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>4501032010</t>
+          <t>4501032100</t>
         </is>
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>P171</t>
+          <t>P327</t>
         </is>
       </c>
       <c r="C110" t="inlineStr">
         <is>
-          <t>E/S WIESSE</t>
+          <t>E/S ZARATE</t>
         </is>
       </c>
       <c r="D110" t="inlineStr">
         <is>
-          <t>Av. El Bosque, San Juan de Lurigancho 15419</t>
+          <t>Av. Malecón Checa, San Juan de Lurigancho 15401</t>
         </is>
       </c>
       <c r="E110" t="inlineStr">
         <is>
-          <t>CANTO GRANDE</t>
+          <t>ZARATE</t>
         </is>
       </c>
       <c r="F110" t="inlineStr">
@@ -7012,53 +7012,53 @@
         </is>
       </c>
       <c r="H110" t="n">
-        <v>2000</v>
+        <v>500</v>
       </c>
       <c r="I110" t="inlineStr">
         <is>
-          <t>40002019</t>
+          <t>40002039</t>
         </is>
       </c>
       <c r="J110" t="inlineStr">
         <is>
-          <t>MAX-D DIESEL B5 S50 UV</t>
+          <t>PRIMAX GASOHOL 90</t>
         </is>
       </c>
       <c r="K110" t="inlineStr">
         <is>
-          <t>P611</t>
+          <t>P614</t>
         </is>
       </c>
       <c r="L110" t="inlineStr">
         <is>
-          <t>TERMINAL REFINERÍA PAMPILLA</t>
+          <t>TERMINAL PBF CALLAO</t>
         </is>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>4501032011</t>
+          <t>4501032101</t>
         </is>
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>P171</t>
+          <t>P327</t>
         </is>
       </c>
       <c r="C111" t="inlineStr">
         <is>
-          <t>E/S WIESSE</t>
+          <t>E/S ZARATE</t>
         </is>
       </c>
       <c r="D111" t="inlineStr">
         <is>
-          <t>Av. El Bosque, San Juan de Lurigancho 15419</t>
+          <t>Av. Malecón Checa, San Juan de Lurigancho 15401</t>
         </is>
       </c>
       <c r="E111" t="inlineStr">
         <is>
-          <t>CANTO GRANDE</t>
+          <t>ZARATE</t>
         </is>
       </c>
       <c r="F111" t="inlineStr">
@@ -7072,7 +7072,7 @@
         </is>
       </c>
       <c r="H111" t="n">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="I111" t="inlineStr">
         <is>
@@ -7086,190 +7086,10 @@
       </c>
       <c r="K111" t="inlineStr">
         <is>
-          <t>P611</t>
+          <t>P614</t>
         </is>
       </c>
       <c r="L111" t="inlineStr">
-        <is>
-          <t>TERMINAL REFINERÍA PAMPILLA</t>
-        </is>
-      </c>
-    </row>
-    <row r="112">
-      <c r="A112" t="inlineStr">
-        <is>
-          <t>4501032011</t>
-        </is>
-      </c>
-      <c r="B112" t="inlineStr">
-        <is>
-          <t>P171</t>
-        </is>
-      </c>
-      <c r="C112" t="inlineStr">
-        <is>
-          <t>E/S WIESSE</t>
-        </is>
-      </c>
-      <c r="D112" t="inlineStr">
-        <is>
-          <t>Av. El Bosque, San Juan de Lurigancho 15419</t>
-        </is>
-      </c>
-      <c r="E112" t="inlineStr">
-        <is>
-          <t>CANTO GRANDE</t>
-        </is>
-      </c>
-      <c r="F112" t="inlineStr">
-        <is>
-          <t>LIMA</t>
-        </is>
-      </c>
-      <c r="G112" t="inlineStr">
-        <is>
-          <t>LIMA</t>
-        </is>
-      </c>
-      <c r="H112" t="n">
-        <v>1000</v>
-      </c>
-      <c r="I112" t="inlineStr">
-        <is>
-          <t>40002047</t>
-        </is>
-      </c>
-      <c r="J112" t="inlineStr">
-        <is>
-          <t>PRIMAX GASOHOL 95</t>
-        </is>
-      </c>
-      <c r="K112" t="inlineStr">
-        <is>
-          <t>P611</t>
-        </is>
-      </c>
-      <c r="L112" t="inlineStr">
-        <is>
-          <t>TERMINAL REFINERÍA PAMPILLA</t>
-        </is>
-      </c>
-    </row>
-    <row r="113">
-      <c r="A113" t="inlineStr">
-        <is>
-          <t>4501032100</t>
-        </is>
-      </c>
-      <c r="B113" t="inlineStr">
-        <is>
-          <t>P327</t>
-        </is>
-      </c>
-      <c r="C113" t="inlineStr">
-        <is>
-          <t>E/S ZARATE</t>
-        </is>
-      </c>
-      <c r="D113" t="inlineStr">
-        <is>
-          <t>Av. Malecón Checa, San Juan de Lurigancho 15401</t>
-        </is>
-      </c>
-      <c r="E113" t="inlineStr">
-        <is>
-          <t>ZARATE</t>
-        </is>
-      </c>
-      <c r="F113" t="inlineStr">
-        <is>
-          <t>LIMA</t>
-        </is>
-      </c>
-      <c r="G113" t="inlineStr">
-        <is>
-          <t>LIMA</t>
-        </is>
-      </c>
-      <c r="H113" t="n">
-        <v>500</v>
-      </c>
-      <c r="I113" t="inlineStr">
-        <is>
-          <t>40002039</t>
-        </is>
-      </c>
-      <c r="J113" t="inlineStr">
-        <is>
-          <t>PRIMAX GASOHOL 90</t>
-        </is>
-      </c>
-      <c r="K113" t="inlineStr">
-        <is>
-          <t>P614</t>
-        </is>
-      </c>
-      <c r="L113" t="inlineStr">
-        <is>
-          <t>TERMINAL PBF CALLAO</t>
-        </is>
-      </c>
-    </row>
-    <row r="114">
-      <c r="A114" t="inlineStr">
-        <is>
-          <t>4501032101</t>
-        </is>
-      </c>
-      <c r="B114" t="inlineStr">
-        <is>
-          <t>P327</t>
-        </is>
-      </c>
-      <c r="C114" t="inlineStr">
-        <is>
-          <t>E/S ZARATE</t>
-        </is>
-      </c>
-      <c r="D114" t="inlineStr">
-        <is>
-          <t>Av. Malecón Checa, San Juan de Lurigancho 15401</t>
-        </is>
-      </c>
-      <c r="E114" t="inlineStr">
-        <is>
-          <t>ZARATE</t>
-        </is>
-      </c>
-      <c r="F114" t="inlineStr">
-        <is>
-          <t>LIMA</t>
-        </is>
-      </c>
-      <c r="G114" t="inlineStr">
-        <is>
-          <t>LIMA</t>
-        </is>
-      </c>
-      <c r="H114" t="n">
-        <v>500</v>
-      </c>
-      <c r="I114" t="inlineStr">
-        <is>
-          <t>40002039</t>
-        </is>
-      </c>
-      <c r="J114" t="inlineStr">
-        <is>
-          <t>PRIMAX GASOHOL 90</t>
-        </is>
-      </c>
-      <c r="K114" t="inlineStr">
-        <is>
-          <t>P614</t>
-        </is>
-      </c>
-      <c r="L114" t="inlineStr">
         <is>
           <t>TERMINAL PBF CALLAO</t>
         </is>

</xml_diff>